<commit_message>
First release of Hello World!
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="428">
   <si>
     <t>Product Name</t>
   </si>
@@ -1473,6 +1473,38 @@
   </si>
   <si>
     <t>it should be successfully Create Sales Quotation</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Checking Item Type drop down option showing same Item Type list in item profile page</t>
+  </si>
+  <si>
+    <t>Configuration-&gt;Item profile-&gt;Item Type-&gt;view</t>
+  </si>
+  <si>
+    <t>Item Type:Raw Material</t>
+  </si>
+  <si>
+    <t>Should be Item Type drop down option showing same Item Type list in item profile page</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Checking SL No Filter in Item profile when switching page</t>
+  </si>
+  <si>
+    <t>Configuration-&gt;Item profile-&gt;Item Type-&gt;view-&gt;Filter button</t>
+  </si>
+  <si>
+    <t>Item Type:Raw Material 
+Range:100 
+Filter: 101-200</t>
+  </si>
+  <si>
+    <t>Should be SL No showing Filter in Item profile when switching page</t>
   </si>
 </sst>
 </file>
@@ -1798,7 +1830,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1901,12 +1933,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2078,30 +2170,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2112,17 +2185,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2139,14 +2206,81 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2369,8 +2503,8 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -2385,232 +2519,232 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="70"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="74" t="s">
+      <c r="E1" s="86"/>
+      <c r="F1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="75">
+      <c r="G1" s="86"/>
+      <c r="H1" s="91">
         <v>45615</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="76" t="s">
+      <c r="I1" s="86"/>
+      <c r="J1" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="72"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78" t="s">
+      <c r="K1" s="86"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
       <c r="P1" s="69"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="13.8">
       <c r="A2" s="70"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73" t="s">
+      <c r="C2" s="86"/>
+      <c r="D2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="74" t="s">
+      <c r="E2" s="86"/>
+      <c r="F2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="80" t="s">
+      <c r="G2" s="86"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="81">
+      <c r="K2" s="74">
         <f>COUNTIF(M8:M1821,"Pass")</f>
-        <v>72</v>
-      </c>
-      <c r="L2" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="13.8">
       <c r="A3" s="70"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="74" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="84" t="s">
+      <c r="G3" s="86"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="85">
+      <c r="K3" s="77">
         <f>COUNTIF(M8:M1821,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="L3" s="82" t="s">
+      <c r="L3" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="171.6">
       <c r="A4" s="70"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="74" t="s">
+      <c r="E4" s="86"/>
+      <c r="F4" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="72"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="80" t="s">
+      <c r="G4" s="86"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="78">
         <f>COUNTIF(M9:M1821,"Out of Scope")</f>
         <v>0</v>
       </c>
-      <c r="L4" s="88" t="s">
+      <c r="L4" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="70"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73" t="s">
+      <c r="C5" s="86"/>
+      <c r="D5" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="74" t="s">
+      <c r="E5" s="86"/>
+      <c r="F5" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="72"/>
-      <c r="H5" s="79" t="s">
+      <c r="G5" s="86"/>
+      <c r="H5" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="72"/>
-      <c r="J5" s="89" t="s">
+      <c r="I5" s="86"/>
+      <c r="J5" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="90">
+      <c r="K5" s="81">
         <f>SUM(K2+K3+K4)</f>
-        <v>72</v>
-      </c>
-      <c r="L5" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="91"/>
-      <c r="B6" s="91"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="92"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="82" t="s">
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="26.4">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="94" t="s">
+      <c r="G7" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="94" t="s">
+      <c r="H7" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="93" t="s">
+      <c r="I7" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="93" t="s">
+      <c r="J7" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="94" t="s">
+      <c r="K7" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="94" t="s">
+      <c r="L7" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="94" t="s">
+      <c r="M7" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="94" t="s">
+      <c r="N7" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="94" t="s">
+      <c r="O7" s="84" t="s">
         <v>39</v>
       </c>
       <c r="P7" s="2"/>
@@ -5649,47 +5783,109 @@
       <c r="Y79" s="36"/>
       <c r="Z79" s="36"/>
     </row>
-    <row r="80" spans="1:26">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
-      <c r="Q80" s="4"/>
-      <c r="R80" s="4"/>
-    </row>
-    <row r="81" spans="1:18">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
-      <c r="R81" s="4"/>
-    </row>
-    <row r="82" spans="1:18">
+    <row r="80" spans="1:26" ht="106.2" thickBot="1">
+      <c r="A80" s="95">
+        <v>45394</v>
+      </c>
+      <c r="B80" s="96" t="s">
+        <v>290</v>
+      </c>
+      <c r="C80" s="96" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="E80" s="98" t="s">
+        <v>418</v>
+      </c>
+      <c r="F80" s="96" t="s">
+        <v>419</v>
+      </c>
+      <c r="G80" s="99" t="s">
+        <v>291</v>
+      </c>
+      <c r="H80" s="96" t="s">
+        <v>420</v>
+      </c>
+      <c r="I80" s="96" t="s">
+        <v>421</v>
+      </c>
+      <c r="J80" s="96"/>
+      <c r="K80" s="96" t="s">
+        <v>422</v>
+      </c>
+      <c r="L80" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="M80" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="N80" s="36"/>
+      <c r="O80" s="36"/>
+      <c r="P80" s="36"/>
+      <c r="Q80" s="36"/>
+      <c r="R80" s="36"/>
+      <c r="S80" s="36"/>
+      <c r="T80" s="36"/>
+      <c r="U80" s="36"/>
+      <c r="V80" s="36"/>
+      <c r="W80" s="36"/>
+      <c r="X80" s="36"/>
+      <c r="Y80" s="36"/>
+      <c r="Z80" s="36"/>
+    </row>
+    <row r="81" spans="1:26" ht="79.8" thickBot="1">
+      <c r="A81" s="102"/>
+      <c r="B81" s="103" t="s">
+        <v>290</v>
+      </c>
+      <c r="C81" s="103" t="s">
+        <v>234</v>
+      </c>
+      <c r="D81" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="105" t="s">
+        <v>423</v>
+      </c>
+      <c r="F81" s="103" t="s">
+        <v>424</v>
+      </c>
+      <c r="G81" s="106" t="s">
+        <v>291</v>
+      </c>
+      <c r="H81" s="103" t="s">
+        <v>425</v>
+      </c>
+      <c r="I81" s="103" t="s">
+        <v>426</v>
+      </c>
+      <c r="J81" s="103"/>
+      <c r="K81" s="103" t="s">
+        <v>427</v>
+      </c>
+      <c r="L81" s="107" t="s">
+        <v>53</v>
+      </c>
+      <c r="M81" s="108" t="s">
+        <v>41</v>
+      </c>
+      <c r="N81" s="36"/>
+      <c r="O81" s="36"/>
+      <c r="P81" s="36"/>
+      <c r="Q81" s="36"/>
+      <c r="R81" s="36"/>
+      <c r="S81" s="36"/>
+      <c r="T81" s="36"/>
+      <c r="U81" s="36"/>
+      <c r="V81" s="36"/>
+      <c r="W81" s="36"/>
+      <c r="X81" s="36"/>
+      <c r="Y81" s="36"/>
+      <c r="Z81" s="36"/>
+    </row>
+    <row r="82" spans="1:26">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -5709,7 +5905,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:26">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -5729,7 +5925,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:26">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -5749,7 +5945,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:26">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -5769,7 +5965,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:26">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -5789,7 +5985,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:26">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -5809,7 +6005,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:26">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -5829,7 +6025,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:26">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -5849,7 +6045,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:26">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -5869,7 +6065,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:26">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -5889,7 +6085,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:26">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -5909,7 +6105,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:26">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -5929,7 +6125,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:26">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -5949,7 +6145,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:26">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -5969,7 +6165,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:26">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -24131,6 +24327,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -24145,14 +24349,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8 M18">

</xml_diff>

<commit_message>
sales reports QTY sales and purchase
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="549">
   <si>
     <t>Product Name</t>
   </si>
@@ -1957,6 +1957,158 @@
   </si>
   <si>
     <t>It should be successfully displays purchase received details when searched using a valid PO number.</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7563</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sales Order</t>
+    </r>
+  </si>
+  <si>
+    <t>Create Sales Order</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Sale-Sales Order-Create Sales Order-fillup form-save</t>
+  </si>
+  <si>
+    <t>Create Date: Enter 12/11/2024. 
+Office: MGM Head Office. 
+Customer: ABDUL MONEM LIMITED (32 125761939) from the dropdown. 
+Ship To: the address Monem Business District 111, Bir Uttam C.R. Dutta Road, Level – 13. 
+Contact To: Enter Akbar 63. 
+Sales Force: Asaduzzaman. 
+Type: Sales. 
+Exp. Delivery Date: Enter 12/11/2024 
+Item- Customer 
+rwetrytytyrtwre - xiamio --0071324456 (PCS) 
+Quantity (PCS) - 3 
+Rate- 8</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7563</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Approval</t>
+    </r>
+  </si>
+  <si>
+    <t>Sales Approval</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify Sales Order Approval Process</t>
+  </si>
+  <si>
+    <t>Approval-Sales Approval-Sales Order Approval-select-Approve-yes</t>
+  </si>
+  <si>
+    <t>It should be successfully Approve Sales Order</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7563</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Purchase Receive</t>
+    </r>
+  </si>
+  <si>
+    <t>Direct Receive / Direct Purchase</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>Try to Direct Receive / Direct Purchase tagging with SO</t>
+  </si>
+  <si>
+    <t>Purchase -Purchase Receive-Direct Receive / Direct Purchase -select Create From Sales Order-fillup form-save</t>
+  </si>
+  <si>
+    <t>Select Create From Sales Order 
+Sales Order- SO-M241200174 
+Customer-ABDUL MONEM LIMITED 
+Office- MGM Head Office 
+Warehouse-MGM Warehouse bd 
+Item Type- Inventory Item 
+Select Supplier - 1234 (2131211) 
+Receive Qty- 8 
+Rate (WST)- 9</t>
+  </si>
+  <si>
+    <t>It should be successfully Direct Receive / Direct Purchase</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>Verify Purchase Received Details showing with PO Number/GRN</t>
+  </si>
+  <si>
+    <t>It should be successfully displays purchase received details when searched using a valid PO number./ GRN</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7563</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sales </t>
+    </r>
+  </si>
+  <si>
+    <t>Sales Report</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>Verify Sales Report Details like:(Sales Qty,Sales Order Amount,Purchase Qty,COGS/Purchase Amount) showing with SO.</t>
+  </si>
+  <si>
+    <t>Sale-Sales Report-View By View By Order Wise Profit/Margin-fillup form-view</t>
+  </si>
+  <si>
+    <t>It should be showing Sales Report Details like:(Sales Qty,Sales Order Amount,Purchase Qty,COGS/Purchase Amount)</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -2470,12 +2622,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2671,34 +2838,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2748,6 +2887,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2971,8 +3156,8 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N103" sqref="N103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -2987,26 +3172,26 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="46"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="80" t="s">
+      <c r="C1" s="95"/>
+      <c r="D1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="81" t="s">
+      <c r="E1" s="95"/>
+      <c r="F1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="83">
+      <c r="G1" s="95"/>
+      <c r="H1" s="103">
         <v>45615</v>
       </c>
-      <c r="I1" s="78"/>
-      <c r="J1" s="77" t="s">
+      <c r="I1" s="95"/>
+      <c r="J1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="78"/>
+      <c r="K1" s="95"/>
       <c r="L1" s="47"/>
       <c r="M1" s="48" t="s">
         <v>4</v>
@@ -3019,26 +3204,26 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="46"/>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="80" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="81" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="78"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="95"/>
       <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="50">
         <f>COUNTIF(M8:M1821,"Pass")</f>
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L2" s="51" t="s">
         <v>9</v>
@@ -3052,16 +3237,16 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="46"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="81" t="s">
+      <c r="B3" s="96"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="78"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="95"/>
       <c r="J3" s="52" t="s">
         <v>11</v>
       </c>
@@ -3081,20 +3266,20 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="46"/>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="80" t="s">
+      <c r="C4" s="95"/>
+      <c r="D4" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="81" t="s">
+      <c r="E4" s="95"/>
+      <c r="F4" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="78"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="95"/>
       <c r="J4" s="49" t="s">
         <v>16</v>
       </c>
@@ -3114,28 +3299,28 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="46"/>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="80" t="s">
+      <c r="C5" s="95"/>
+      <c r="D5" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="81" t="s">
+      <c r="E5" s="95"/>
+      <c r="F5" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="78"/>
-      <c r="H5" s="82" t="s">
+      <c r="G5" s="95"/>
+      <c r="H5" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="78"/>
+      <c r="I5" s="95"/>
       <c r="J5" s="56" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="57">
         <f>SUM(K2+K3+K4)</f>
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L5" s="51" t="s">
         <v>23</v>
@@ -3150,14 +3335,14 @@
     <row r="6" spans="1:26">
       <c r="A6" s="58"/>
       <c r="B6" s="58"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
       <c r="K6" s="58"/>
       <c r="L6" s="51" t="s">
         <v>24</v>
@@ -3244,13 +3429,13 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="159" thickBot="1">
-      <c r="A9" s="87">
+      <c r="A9" s="77">
         <v>45615</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="78" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="62" t="s">
@@ -3271,10 +3456,10 @@
       <c r="I9" s="61" t="s">
         <v>452</v>
       </c>
-      <c r="J9" s="89" t="s">
+      <c r="J9" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="90" t="s">
+      <c r="K9" s="80" t="s">
         <v>49</v>
       </c>
       <c r="L9" s="61" t="s">
@@ -3283,8 +3468,8 @@
       <c r="M9" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
       <c r="R9" s="36"/>
@@ -3299,10 +3484,10 @@
     </row>
     <row r="10" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A10" s="66"/>
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="82" t="s">
         <v>453</v>
       </c>
       <c r="D10" s="68" t="s">
@@ -3322,7 +3507,7 @@
         <v>53</v>
       </c>
       <c r="J10" s="67"/>
-      <c r="K10" s="93" t="s">
+      <c r="K10" s="83" t="s">
         <v>54</v>
       </c>
       <c r="L10" s="67" t="s">
@@ -3347,10 +3532,10 @@
     </row>
     <row r="11" spans="1:26" ht="132.6" thickBot="1">
       <c r="A11" s="66"/>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="82" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="68" t="s">
@@ -3374,7 +3559,7 @@
       <c r="J11" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="93" t="s">
+      <c r="K11" s="83" t="s">
         <v>60</v>
       </c>
       <c r="L11" s="67" t="s">
@@ -3399,10 +3584,10 @@
     </row>
     <row r="12" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A12" s="66"/>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="82" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="68" t="s">
@@ -3424,7 +3609,7 @@
         <v>53</v>
       </c>
       <c r="J12" s="67"/>
-      <c r="K12" s="93" t="s">
+      <c r="K12" s="83" t="s">
         <v>66</v>
       </c>
       <c r="L12" s="67" t="s">
@@ -3449,10 +3634,10 @@
     </row>
     <row r="13" spans="1:26" ht="119.4" thickBot="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="92" t="s">
+      <c r="C13" s="82" t="s">
         <v>61</v>
       </c>
       <c r="D13" s="68" t="s">
@@ -3476,7 +3661,7 @@
       <c r="J13" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="K13" s="93" t="s">
+      <c r="K13" s="83" t="s">
         <v>72</v>
       </c>
       <c r="L13" s="67" t="s">
@@ -3501,10 +3686,10 @@
     </row>
     <row r="14" spans="1:26" ht="132.6" thickBot="1">
       <c r="A14" s="66"/>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="92" t="s">
+      <c r="C14" s="82" t="s">
         <v>61</v>
       </c>
       <c r="D14" s="68" t="s">
@@ -3528,7 +3713,7 @@
       <c r="J14" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="93" t="s">
+      <c r="K14" s="83" t="s">
         <v>77</v>
       </c>
       <c r="L14" s="67" t="s">
@@ -3553,10 +3738,10 @@
     </row>
     <row r="15" spans="1:26" ht="119.4" thickBot="1">
       <c r="A15" s="66"/>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="82" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="68" t="s">
@@ -3580,7 +3765,7 @@
       <c r="J15" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="93" t="s">
+      <c r="K15" s="83" t="s">
         <v>455</v>
       </c>
       <c r="L15" s="67" t="s">
@@ -3605,10 +3790,10 @@
     </row>
     <row r="16" spans="1:26" ht="119.4" thickBot="1">
       <c r="A16" s="66"/>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="82" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="68" t="s">
@@ -3659,10 +3844,10 @@
       <c r="A17" s="73">
         <v>45617</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="92" t="s">
+      <c r="C17" s="82" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="68" t="s">
@@ -3711,7 +3896,7 @@
     </row>
     <row r="18" spans="1:26" ht="14.4" thickBot="1">
       <c r="A18" s="66"/>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="82" t="s">
         <v>94</v>
       </c>
       <c r="C18" s="67"/>
@@ -3747,10 +3932,10 @@
     </row>
     <row r="19" spans="1:26" ht="409.6" thickBot="1">
       <c r="A19" s="66"/>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="92" t="s">
+      <c r="C19" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="68" t="s">
@@ -3799,10 +3984,10 @@
     </row>
     <row r="20" spans="1:26" ht="53.4" thickBot="1">
       <c r="A20" s="66"/>
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="92" t="s">
+      <c r="C20" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D20" s="68" t="s">
@@ -3849,10 +4034,10 @@
     </row>
     <row r="21" spans="1:26" ht="53.4" thickBot="1">
       <c r="A21" s="66"/>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D21" s="68" t="s">
@@ -3901,10 +4086,10 @@
     </row>
     <row r="22" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A22" s="66"/>
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="92" t="s">
+      <c r="C22" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D22" s="68" t="s">
@@ -3953,10 +4138,10 @@
     </row>
     <row r="23" spans="1:26" ht="93" thickBot="1">
       <c r="A23" s="66"/>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="92" t="s">
+      <c r="C23" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D23" s="68" t="s">
@@ -4005,10 +4190,10 @@
     </row>
     <row r="24" spans="1:26" ht="53.4" thickBot="1">
       <c r="A24" s="66"/>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D24" s="68" t="s">
@@ -4057,10 +4242,10 @@
     </row>
     <row r="25" spans="1:26" ht="93" thickBot="1">
       <c r="A25" s="66"/>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D25" s="68" t="s">
@@ -4109,10 +4294,10 @@
     </row>
     <row r="26" spans="1:26" ht="170.4" customHeight="1" thickBot="1">
       <c r="A26" s="66"/>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="82" t="s">
         <v>295</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="82" t="s">
         <v>130</v>
       </c>
       <c r="D26" s="68" t="s">
@@ -4161,10 +4346,10 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" thickBot="1">
       <c r="A27" s="66"/>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="82" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="92" t="s">
+      <c r="C27" s="82" t="s">
         <v>130</v>
       </c>
       <c r="D27" s="68" t="s">
@@ -4204,7 +4389,7 @@
     <row r="28" spans="1:26" ht="14.4" thickBot="1">
       <c r="A28" s="66"/>
       <c r="B28" s="67"/>
-      <c r="C28" s="92" t="s">
+      <c r="C28" s="82" t="s">
         <v>139</v>
       </c>
       <c r="D28" s="67"/>
@@ -4237,7 +4422,7 @@
     </row>
     <row r="29" spans="1:26" ht="79.8" thickBot="1">
       <c r="A29" s="66"/>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="82" t="s">
         <v>141</v>
       </c>
       <c r="C29" s="67"/>
@@ -4257,8 +4442,8 @@
       <c r="M29" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="N29" s="94"/>
-      <c r="O29" s="94"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="84"/>
       <c r="P29" s="36"/>
       <c r="Q29" s="36"/>
       <c r="R29" s="36"/>
@@ -4272,14 +4457,14 @@
       <c r="Z29" s="36"/>
     </row>
     <row r="30" spans="1:26" ht="238.8" thickBot="1">
-      <c r="A30" s="95"/>
-      <c r="B30" s="96" t="s">
+      <c r="A30" s="85"/>
+      <c r="B30" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="C30" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="97" t="s">
+      <c r="D30" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="69" t="s">
@@ -4288,7 +4473,7 @@
       <c r="F30" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="98" t="s">
+      <c r="G30" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H30" s="71" t="s">
@@ -4297,7 +4482,7 @@
       <c r="I30" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="J30" s="99" t="s">
+      <c r="J30" s="89" t="s">
         <v>149</v>
       </c>
       <c r="K30" s="71" t="s">
@@ -4306,32 +4491,32 @@
       <c r="L30" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M30" s="100" t="s">
+      <c r="M30" s="90" t="s">
         <v>41</v>
       </c>
       <c r="N30" s="71"/>
       <c r="O30" s="71"/>
-      <c r="P30" s="101"/>
-      <c r="Q30" s="101"/>
-      <c r="R30" s="101"/>
-      <c r="S30" s="101"/>
-      <c r="T30" s="101"/>
-      <c r="U30" s="101"/>
-      <c r="V30" s="101"/>
-      <c r="W30" s="101"/>
-      <c r="X30" s="101"/>
-      <c r="Y30" s="101"/>
-      <c r="Z30" s="101"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="91"/>
+      <c r="R30" s="91"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="91"/>
+      <c r="X30" s="91"/>
+      <c r="Y30" s="91"/>
+      <c r="Z30" s="91"/>
     </row>
     <row r="31" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A31" s="102"/>
-      <c r="B31" s="96" t="s">
+      <c r="A31" s="92"/>
+      <c r="B31" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="96" t="s">
+      <c r="C31" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="97" t="s">
+      <c r="D31" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="69" t="s">
@@ -4340,7 +4525,7 @@
       <c r="F31" s="67" t="s">
         <v>459</v>
       </c>
-      <c r="G31" s="103" t="s">
+      <c r="G31" s="93" t="s">
         <v>64</v>
       </c>
       <c r="H31" s="71" t="s">
@@ -4349,41 +4534,41 @@
       <c r="I31" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="99" t="s">
+      <c r="J31" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="K31" s="102" t="s">
+      <c r="K31" s="92" t="s">
         <v>154</v>
       </c>
       <c r="L31" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M31" s="100" t="s">
+      <c r="M31" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N31" s="101"/>
-      <c r="O31" s="101"/>
-      <c r="P31" s="101"/>
-      <c r="Q31" s="101"/>
-      <c r="R31" s="101"/>
-      <c r="S31" s="101"/>
-      <c r="T31" s="101"/>
-      <c r="U31" s="101"/>
-      <c r="V31" s="101"/>
-      <c r="W31" s="101"/>
-      <c r="X31" s="101"/>
-      <c r="Y31" s="101"/>
-      <c r="Z31" s="101"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="91"/>
+      <c r="P31" s="91"/>
+      <c r="Q31" s="91"/>
+      <c r="R31" s="91"/>
+      <c r="S31" s="91"/>
+      <c r="T31" s="91"/>
+      <c r="U31" s="91"/>
+      <c r="V31" s="91"/>
+      <c r="W31" s="91"/>
+      <c r="X31" s="91"/>
+      <c r="Y31" s="91"/>
+      <c r="Z31" s="91"/>
     </row>
     <row r="32" spans="1:26" ht="67.2" thickBot="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="96" t="s">
+      <c r="A32" s="92"/>
+      <c r="B32" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="96" t="s">
+      <c r="C32" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="97" t="s">
+      <c r="D32" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="69" t="s">
@@ -4392,7 +4577,7 @@
       <c r="F32" s="71" t="s">
         <v>156</v>
       </c>
-      <c r="G32" s="98" t="s">
+      <c r="G32" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H32" s="71" t="s">
@@ -4401,7 +4586,7 @@
       <c r="I32" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="J32" s="99" t="s">
+      <c r="J32" s="89" t="s">
         <v>159</v>
       </c>
       <c r="K32" s="71" t="s">
@@ -4410,32 +4595,32 @@
       <c r="L32" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M32" s="100" t="s">
+      <c r="M32" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
-      <c r="P32" s="101"/>
-      <c r="Q32" s="101"/>
-      <c r="R32" s="101"/>
-      <c r="S32" s="101"/>
-      <c r="T32" s="101"/>
-      <c r="U32" s="101"/>
-      <c r="V32" s="101"/>
-      <c r="W32" s="101"/>
-      <c r="X32" s="101"/>
-      <c r="Y32" s="101"/>
-      <c r="Z32" s="101"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="91"/>
+      <c r="P32" s="91"/>
+      <c r="Q32" s="91"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="91"/>
+      <c r="T32" s="91"/>
+      <c r="U32" s="91"/>
+      <c r="V32" s="91"/>
+      <c r="W32" s="91"/>
+      <c r="X32" s="91"/>
+      <c r="Y32" s="91"/>
+      <c r="Z32" s="91"/>
     </row>
     <row r="33" spans="1:26" ht="133.19999999999999" thickBot="1">
-      <c r="A33" s="102"/>
-      <c r="B33" s="96" t="s">
+      <c r="A33" s="92"/>
+      <c r="B33" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="96" t="s">
+      <c r="C33" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="97" t="s">
+      <c r="D33" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="69" t="s">
@@ -4444,7 +4629,7 @@
       <c r="F33" s="71" t="s">
         <v>460</v>
       </c>
-      <c r="G33" s="98" t="s">
+      <c r="G33" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H33" s="71" t="s">
@@ -4458,32 +4643,32 @@
       <c r="L33" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M33" s="100" t="s">
+      <c r="M33" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N33" s="101"/>
-      <c r="O33" s="101"/>
-      <c r="P33" s="101"/>
-      <c r="Q33" s="101"/>
-      <c r="R33" s="101"/>
-      <c r="S33" s="101"/>
-      <c r="T33" s="101"/>
-      <c r="U33" s="101"/>
-      <c r="V33" s="101"/>
-      <c r="W33" s="101"/>
-      <c r="X33" s="101"/>
-      <c r="Y33" s="101"/>
-      <c r="Z33" s="101"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="91"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="91"/>
+      <c r="R33" s="91"/>
+      <c r="S33" s="91"/>
+      <c r="T33" s="91"/>
+      <c r="U33" s="91"/>
+      <c r="V33" s="91"/>
+      <c r="W33" s="91"/>
+      <c r="X33" s="91"/>
+      <c r="Y33" s="91"/>
+      <c r="Z33" s="91"/>
     </row>
     <row r="34" spans="1:26" ht="133.19999999999999" thickBot="1">
-      <c r="A34" s="102"/>
-      <c r="B34" s="96" t="s">
+      <c r="A34" s="92"/>
+      <c r="B34" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="96" t="s">
+      <c r="C34" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="97" t="s">
+      <c r="D34" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E34" s="69" t="s">
@@ -4492,7 +4677,7 @@
       <c r="F34" s="71" t="s">
         <v>461</v>
       </c>
-      <c r="G34" s="98" t="s">
+      <c r="G34" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H34" s="71" t="s">
@@ -4506,32 +4691,32 @@
       <c r="L34" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M34" s="100" t="s">
+      <c r="M34" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N34" s="101"/>
-      <c r="O34" s="101"/>
-      <c r="P34" s="101"/>
-      <c r="Q34" s="101"/>
-      <c r="R34" s="101"/>
-      <c r="S34" s="101"/>
-      <c r="T34" s="101"/>
-      <c r="U34" s="101"/>
-      <c r="V34" s="101"/>
-      <c r="W34" s="101"/>
-      <c r="X34" s="101"/>
-      <c r="Y34" s="101"/>
-      <c r="Z34" s="101"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="91"/>
+      <c r="P34" s="91"/>
+      <c r="Q34" s="91"/>
+      <c r="R34" s="91"/>
+      <c r="S34" s="91"/>
+      <c r="T34" s="91"/>
+      <c r="U34" s="91"/>
+      <c r="V34" s="91"/>
+      <c r="W34" s="91"/>
+      <c r="X34" s="91"/>
+      <c r="Y34" s="91"/>
+      <c r="Z34" s="91"/>
     </row>
     <row r="35" spans="1:26" ht="80.400000000000006" thickBot="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="96" t="s">
+      <c r="A35" s="92"/>
+      <c r="B35" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="96" t="s">
+      <c r="C35" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="97" t="s">
+      <c r="D35" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E35" s="69" t="s">
@@ -4540,7 +4725,7 @@
       <c r="F35" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="G35" s="103" t="s">
+      <c r="G35" s="93" t="s">
         <v>64</v>
       </c>
       <c r="H35" s="71" t="s">
@@ -4549,7 +4734,7 @@
       <c r="I35" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="J35" s="99" t="s">
+      <c r="J35" s="89" t="s">
         <v>167</v>
       </c>
       <c r="K35" s="71" t="s">
@@ -4558,32 +4743,32 @@
       <c r="L35" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M35" s="100" t="s">
+      <c r="M35" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N35" s="101"/>
-      <c r="O35" s="101"/>
-      <c r="P35" s="101"/>
-      <c r="Q35" s="101"/>
-      <c r="R35" s="101"/>
-      <c r="S35" s="101"/>
-      <c r="T35" s="101"/>
-      <c r="U35" s="101"/>
-      <c r="V35" s="101"/>
-      <c r="W35" s="101"/>
-      <c r="X35" s="101"/>
-      <c r="Y35" s="101"/>
-      <c r="Z35" s="101"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="91"/>
+      <c r="P35" s="91"/>
+      <c r="Q35" s="91"/>
+      <c r="R35" s="91"/>
+      <c r="S35" s="91"/>
+      <c r="T35" s="91"/>
+      <c r="U35" s="91"/>
+      <c r="V35" s="91"/>
+      <c r="W35" s="91"/>
+      <c r="X35" s="91"/>
+      <c r="Y35" s="91"/>
+      <c r="Z35" s="91"/>
     </row>
     <row r="36" spans="1:26" ht="80.400000000000006" thickBot="1">
-      <c r="A36" s="102"/>
-      <c r="B36" s="96" t="s">
+      <c r="A36" s="92"/>
+      <c r="B36" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="96" t="s">
+      <c r="C36" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="97" t="s">
+      <c r="D36" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E36" s="69" t="s">
@@ -4592,7 +4777,7 @@
       <c r="F36" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="G36" s="103" t="s">
+      <c r="G36" s="93" t="s">
         <v>64</v>
       </c>
       <c r="H36" s="71" t="s">
@@ -4608,32 +4793,32 @@
       <c r="L36" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M36" s="100" t="s">
+      <c r="M36" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N36" s="101"/>
-      <c r="O36" s="101"/>
-      <c r="P36" s="101"/>
-      <c r="Q36" s="101"/>
-      <c r="R36" s="101"/>
-      <c r="S36" s="101"/>
-      <c r="T36" s="101"/>
-      <c r="U36" s="101"/>
-      <c r="V36" s="101"/>
-      <c r="W36" s="101"/>
-      <c r="X36" s="101"/>
-      <c r="Y36" s="101"/>
-      <c r="Z36" s="101"/>
+      <c r="N36" s="91"/>
+      <c r="O36" s="91"/>
+      <c r="P36" s="91"/>
+      <c r="Q36" s="91"/>
+      <c r="R36" s="91"/>
+      <c r="S36" s="91"/>
+      <c r="T36" s="91"/>
+      <c r="U36" s="91"/>
+      <c r="V36" s="91"/>
+      <c r="W36" s="91"/>
+      <c r="X36" s="91"/>
+      <c r="Y36" s="91"/>
+      <c r="Z36" s="91"/>
     </row>
     <row r="37" spans="1:26" ht="93.6" thickBot="1">
-      <c r="A37" s="102"/>
-      <c r="B37" s="96" t="s">
+      <c r="A37" s="92"/>
+      <c r="B37" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="96" t="s">
+      <c r="C37" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="D37" s="97" t="s">
+      <c r="D37" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="69" t="s">
@@ -4642,7 +4827,7 @@
       <c r="F37" s="71" t="s">
         <v>464</v>
       </c>
-      <c r="G37" s="98" t="s">
+      <c r="G37" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H37" s="71" t="s">
@@ -4658,32 +4843,32 @@
       <c r="L37" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M37" s="100" t="s">
+      <c r="M37" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N37" s="101"/>
-      <c r="O37" s="101"/>
-      <c r="P37" s="101"/>
-      <c r="Q37" s="101"/>
-      <c r="R37" s="101"/>
-      <c r="S37" s="101"/>
-      <c r="T37" s="101"/>
-      <c r="U37" s="101"/>
-      <c r="V37" s="101"/>
-      <c r="W37" s="101"/>
-      <c r="X37" s="101"/>
-      <c r="Y37" s="101"/>
-      <c r="Z37" s="101"/>
+      <c r="N37" s="91"/>
+      <c r="O37" s="91"/>
+      <c r="P37" s="91"/>
+      <c r="Q37" s="91"/>
+      <c r="R37" s="91"/>
+      <c r="S37" s="91"/>
+      <c r="T37" s="91"/>
+      <c r="U37" s="91"/>
+      <c r="V37" s="91"/>
+      <c r="W37" s="91"/>
+      <c r="X37" s="91"/>
+      <c r="Y37" s="91"/>
+      <c r="Z37" s="91"/>
     </row>
     <row r="38" spans="1:26" ht="93.6" thickBot="1">
-      <c r="A38" s="102"/>
-      <c r="B38" s="96" t="s">
+      <c r="A38" s="92"/>
+      <c r="B38" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="C38" s="96" t="s">
+      <c r="C38" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="D38" s="97" t="s">
+      <c r="D38" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="69" t="s">
@@ -4692,7 +4877,7 @@
       <c r="F38" s="71" t="s">
         <v>466</v>
       </c>
-      <c r="G38" s="98" t="s">
+      <c r="G38" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H38" s="71" t="s">
@@ -4701,7 +4886,7 @@
       <c r="I38" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="J38" s="99" t="s">
+      <c r="J38" s="89" t="s">
         <v>177</v>
       </c>
       <c r="K38" s="71" t="s">
@@ -4710,32 +4895,32 @@
       <c r="L38" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M38" s="100" t="s">
+      <c r="M38" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N38" s="101"/>
-      <c r="O38" s="101"/>
-      <c r="P38" s="101"/>
-      <c r="Q38" s="101"/>
-      <c r="R38" s="101"/>
-      <c r="S38" s="101"/>
-      <c r="T38" s="101"/>
-      <c r="U38" s="101"/>
-      <c r="V38" s="101"/>
-      <c r="W38" s="101"/>
-      <c r="X38" s="101"/>
-      <c r="Y38" s="101"/>
-      <c r="Z38" s="101"/>
+      <c r="N38" s="91"/>
+      <c r="O38" s="91"/>
+      <c r="P38" s="91"/>
+      <c r="Q38" s="91"/>
+      <c r="R38" s="91"/>
+      <c r="S38" s="91"/>
+      <c r="T38" s="91"/>
+      <c r="U38" s="91"/>
+      <c r="V38" s="91"/>
+      <c r="W38" s="91"/>
+      <c r="X38" s="91"/>
+      <c r="Y38" s="91"/>
+      <c r="Z38" s="91"/>
     </row>
     <row r="39" spans="1:26" ht="120" thickBot="1">
-      <c r="A39" s="102"/>
-      <c r="B39" s="96" t="s">
+      <c r="A39" s="92"/>
+      <c r="B39" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="96" t="s">
+      <c r="C39" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="D39" s="97" t="s">
+      <c r="D39" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="69" t="s">
@@ -4744,7 +4929,7 @@
       <c r="F39" s="71" t="s">
         <v>179</v>
       </c>
-      <c r="G39" s="98" t="s">
+      <c r="G39" s="88" t="s">
         <v>264</v>
       </c>
       <c r="H39" s="71" t="s">
@@ -4753,7 +4938,7 @@
       <c r="I39" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="99" t="s">
+      <c r="J39" s="89" t="s">
         <v>181</v>
       </c>
       <c r="K39" s="71" t="s">
@@ -4762,32 +4947,32 @@
       <c r="L39" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M39" s="100" t="s">
+      <c r="M39" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N39" s="101"/>
-      <c r="O39" s="101"/>
-      <c r="P39" s="101"/>
-      <c r="Q39" s="101"/>
-      <c r="R39" s="101"/>
-      <c r="S39" s="101"/>
-      <c r="T39" s="101"/>
-      <c r="U39" s="101"/>
-      <c r="V39" s="101"/>
-      <c r="W39" s="101"/>
-      <c r="X39" s="101"/>
-      <c r="Y39" s="101"/>
-      <c r="Z39" s="101"/>
+      <c r="N39" s="91"/>
+      <c r="O39" s="91"/>
+      <c r="P39" s="91"/>
+      <c r="Q39" s="91"/>
+      <c r="R39" s="91"/>
+      <c r="S39" s="91"/>
+      <c r="T39" s="91"/>
+      <c r="U39" s="91"/>
+      <c r="V39" s="91"/>
+      <c r="W39" s="91"/>
+      <c r="X39" s="91"/>
+      <c r="Y39" s="91"/>
+      <c r="Z39" s="91"/>
     </row>
     <row r="40" spans="1:26" ht="67.2" thickBot="1">
-      <c r="A40" s="102"/>
-      <c r="B40" s="96" t="s">
+      <c r="A40" s="92"/>
+      <c r="B40" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C40" s="96" t="s">
+      <c r="C40" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D40" s="97" t="s">
+      <c r="D40" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="69" t="s">
@@ -4796,7 +4981,7 @@
       <c r="F40" s="71" t="s">
         <v>184</v>
       </c>
-      <c r="G40" s="103" t="s">
+      <c r="G40" s="93" t="s">
         <v>64</v>
       </c>
       <c r="H40" s="71" t="s">
@@ -4805,7 +4990,7 @@
       <c r="I40" s="71" t="s">
         <v>186</v>
       </c>
-      <c r="J40" s="99" t="s">
+      <c r="J40" s="89" t="s">
         <v>187</v>
       </c>
       <c r="K40" s="71" t="s">
@@ -4814,32 +4999,32 @@
       <c r="L40" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M40" s="100" t="s">
+      <c r="M40" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N40" s="101"/>
-      <c r="O40" s="101"/>
-      <c r="P40" s="101"/>
-      <c r="Q40" s="101"/>
-      <c r="R40" s="101"/>
-      <c r="S40" s="101"/>
-      <c r="T40" s="101"/>
-      <c r="U40" s="101"/>
-      <c r="V40" s="101"/>
-      <c r="W40" s="101"/>
-      <c r="X40" s="101"/>
-      <c r="Y40" s="101"/>
-      <c r="Z40" s="101"/>
+      <c r="N40" s="91"/>
+      <c r="O40" s="91"/>
+      <c r="P40" s="91"/>
+      <c r="Q40" s="91"/>
+      <c r="R40" s="91"/>
+      <c r="S40" s="91"/>
+      <c r="T40" s="91"/>
+      <c r="U40" s="91"/>
+      <c r="V40" s="91"/>
+      <c r="W40" s="91"/>
+      <c r="X40" s="91"/>
+      <c r="Y40" s="91"/>
+      <c r="Z40" s="91"/>
     </row>
     <row r="41" spans="1:26" ht="93.6" thickBot="1">
       <c r="A41" s="71"/>
-      <c r="B41" s="96" t="s">
+      <c r="B41" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="96" t="s">
+      <c r="C41" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="97" t="s">
+      <c r="D41" s="87" t="s">
         <v>44</v>
       </c>
       <c r="E41" s="69" t="s">
@@ -4848,7 +5033,7 @@
       <c r="F41" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="G41" s="103" t="s">
+      <c r="G41" s="93" t="s">
         <v>64</v>
       </c>
       <c r="H41" s="71" t="s">
@@ -4857,7 +5042,7 @@
       <c r="I41" s="71" t="s">
         <v>186</v>
       </c>
-      <c r="J41" s="99" t="s">
+      <c r="J41" s="89" t="s">
         <v>192</v>
       </c>
       <c r="K41" s="71" t="s">
@@ -4866,28 +5051,28 @@
       <c r="L41" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M41" s="100" t="s">
+      <c r="M41" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N41" s="101"/>
-      <c r="O41" s="101"/>
-      <c r="P41" s="101"/>
-      <c r="Q41" s="101"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="101"/>
-      <c r="T41" s="101"/>
-      <c r="U41" s="101"/>
-      <c r="V41" s="101"/>
-      <c r="W41" s="101"/>
-      <c r="X41" s="101"/>
-      <c r="Y41" s="101"/>
-      <c r="Z41" s="101"/>
+      <c r="N41" s="91"/>
+      <c r="O41" s="91"/>
+      <c r="P41" s="91"/>
+      <c r="Q41" s="91"/>
+      <c r="R41" s="91"/>
+      <c r="S41" s="91"/>
+      <c r="T41" s="91"/>
+      <c r="U41" s="91"/>
+      <c r="V41" s="91"/>
+      <c r="W41" s="91"/>
+      <c r="X41" s="91"/>
+      <c r="Y41" s="91"/>
+      <c r="Z41" s="91"/>
     </row>
     <row r="42" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A42" s="73">
         <v>45620</v>
       </c>
-      <c r="B42" s="92" t="s">
+      <c r="B42" s="82" t="s">
         <v>194</v>
       </c>
       <c r="C42" s="67"/>
@@ -4919,10 +5104,10 @@
     </row>
     <row r="43" spans="1:26" ht="132.6" thickBot="1">
       <c r="A43" s="66"/>
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="82" t="s">
         <v>337</v>
       </c>
       <c r="D43" s="68" t="s">
@@ -4971,10 +5156,10 @@
     </row>
     <row r="44" spans="1:26" ht="198.6" thickBot="1">
       <c r="A44" s="66"/>
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C44" s="92" t="s">
+      <c r="C44" s="82" t="s">
         <v>469</v>
       </c>
       <c r="D44" s="68" t="s">
@@ -5023,10 +5208,10 @@
     </row>
     <row r="45" spans="1:26" ht="119.4" thickBot="1">
       <c r="A45" s="66"/>
-      <c r="B45" s="92" t="s">
+      <c r="B45" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C45" s="92" t="s">
+      <c r="C45" s="82" t="s">
         <v>207</v>
       </c>
       <c r="D45" s="68" t="s">
@@ -5075,10 +5260,10 @@
     </row>
     <row r="46" spans="1:26" ht="119.4" thickBot="1">
       <c r="A46" s="66"/>
-      <c r="B46" s="92" t="s">
+      <c r="B46" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C46" s="92" t="s">
+      <c r="C46" s="82" t="s">
         <v>207</v>
       </c>
       <c r="D46" s="68" t="s">
@@ -5129,10 +5314,10 @@
       <c r="A47" s="73">
         <v>45628</v>
       </c>
-      <c r="B47" s="92" t="s">
+      <c r="B47" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C47" s="92" t="s">
+      <c r="C47" s="82" t="s">
         <v>207</v>
       </c>
       <c r="D47" s="68" t="s">
@@ -5179,10 +5364,10 @@
     </row>
     <row r="48" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A48" s="66"/>
-      <c r="B48" s="92" t="s">
+      <c r="B48" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C48" s="92" t="s">
+      <c r="C48" s="82" t="s">
         <v>207</v>
       </c>
       <c r="D48" s="68" t="s">
@@ -5229,10 +5414,10 @@
     </row>
     <row r="49" spans="1:26" ht="251.4" thickBot="1">
       <c r="A49" s="66"/>
-      <c r="B49" s="92" t="s">
+      <c r="B49" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="C49" s="92" t="s">
+      <c r="C49" s="82" t="s">
         <v>274</v>
       </c>
       <c r="D49" s="68" t="s">
@@ -5279,10 +5464,10 @@
     </row>
     <row r="50" spans="1:26" ht="79.8" thickBot="1">
       <c r="A50" s="66"/>
-      <c r="B50" s="92" t="s">
+      <c r="B50" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="C50" s="92" t="s">
+      <c r="C50" s="82" t="s">
         <v>274</v>
       </c>
       <c r="D50" s="68" t="s">
@@ -5329,10 +5514,10 @@
     </row>
     <row r="51" spans="1:26" ht="79.8" thickBot="1">
       <c r="A51" s="66"/>
-      <c r="B51" s="92" t="s">
+      <c r="B51" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="C51" s="92" t="s">
+      <c r="C51" s="82" t="s">
         <v>283</v>
       </c>
       <c r="D51" s="68" t="s">
@@ -5379,10 +5564,10 @@
     </row>
     <row r="52" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A52" s="66"/>
-      <c r="B52" s="92" t="s">
+      <c r="B52" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="C52" s="92" t="s">
+      <c r="C52" s="82" t="s">
         <v>283</v>
       </c>
       <c r="D52" s="68" t="s">
@@ -5427,10 +5612,10 @@
     </row>
     <row r="53" spans="1:26" ht="79.8" thickBot="1">
       <c r="A53" s="66"/>
-      <c r="B53" s="92" t="s">
+      <c r="B53" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="92" t="s">
+      <c r="C53" s="82" t="s">
         <v>291</v>
       </c>
       <c r="D53" s="68" t="s">
@@ -5475,10 +5660,10 @@
     </row>
     <row r="54" spans="1:26" ht="343.8" thickBot="1">
       <c r="A54" s="66"/>
-      <c r="B54" s="92" t="s">
+      <c r="B54" s="82" t="s">
         <v>295</v>
       </c>
-      <c r="C54" s="92" t="s">
+      <c r="C54" s="82" t="s">
         <v>296</v>
       </c>
       <c r="D54" s="68" t="s">
@@ -5525,10 +5710,10 @@
     </row>
     <row r="55" spans="1:26" ht="53.4" thickBot="1">
       <c r="A55" s="66"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="82" t="s">
         <v>295</v>
       </c>
-      <c r="C55" s="92" t="s">
+      <c r="C55" s="82" t="s">
         <v>296</v>
       </c>
       <c r="D55" s="68" t="s">
@@ -5575,10 +5760,10 @@
     </row>
     <row r="56" spans="1:26" ht="172.2" thickBot="1">
       <c r="A56" s="66"/>
-      <c r="B56" s="92" t="s">
+      <c r="B56" s="82" t="s">
         <v>295</v>
       </c>
-      <c r="C56" s="92" t="s">
+      <c r="C56" s="82" t="s">
         <v>305</v>
       </c>
       <c r="D56" s="68" t="s">
@@ -5625,10 +5810,10 @@
     </row>
     <row r="57" spans="1:26" ht="53.4" thickBot="1">
       <c r="A57" s="66"/>
-      <c r="B57" s="92" t="s">
+      <c r="B57" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="C57" s="92" t="s">
+      <c r="C57" s="82" t="s">
         <v>309</v>
       </c>
       <c r="D57" s="68" t="s">
@@ -5673,10 +5858,10 @@
     </row>
     <row r="58" spans="1:26" ht="211.8" thickBot="1">
       <c r="A58" s="66"/>
-      <c r="B58" s="92" t="s">
+      <c r="B58" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C58" s="92" t="s">
+      <c r="C58" s="82" t="s">
         <v>313</v>
       </c>
       <c r="D58" s="68" t="s">
@@ -5723,10 +5908,10 @@
     </row>
     <row r="59" spans="1:26" ht="106.2" thickBot="1">
       <c r="A59" s="66"/>
-      <c r="B59" s="92" t="s">
+      <c r="B59" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="C59" s="92" t="s">
+      <c r="C59" s="82" t="s">
         <v>318</v>
       </c>
       <c r="D59" s="68" t="s">
@@ -5773,10 +5958,10 @@
     </row>
     <row r="60" spans="1:26" ht="291" thickBot="1">
       <c r="A60" s="66"/>
-      <c r="B60" s="92" t="s">
+      <c r="B60" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C60" s="92" t="s">
+      <c r="C60" s="82" t="s">
         <v>323</v>
       </c>
       <c r="D60" s="68" t="s">
@@ -5823,10 +6008,10 @@
     </row>
     <row r="61" spans="1:26" ht="251.4" thickBot="1">
       <c r="A61" s="66"/>
-      <c r="B61" s="92" t="s">
+      <c r="B61" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C61" s="92" t="s">
+      <c r="C61" s="82" t="s">
         <v>328</v>
       </c>
       <c r="D61" s="68" t="s">
@@ -5873,10 +6058,10 @@
     </row>
     <row r="62" spans="1:26" ht="79.8" thickBot="1">
       <c r="A62" s="66"/>
-      <c r="B62" s="92" t="s">
+      <c r="B62" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="C62" s="92" t="s">
+      <c r="C62" s="82" t="s">
         <v>333</v>
       </c>
       <c r="D62" s="68" t="s">
@@ -5921,10 +6106,10 @@
     </row>
     <row r="63" spans="1:26" ht="106.2" thickBot="1">
       <c r="A63" s="66"/>
-      <c r="B63" s="92" t="s">
+      <c r="B63" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C63" s="92" t="s">
+      <c r="C63" s="82" t="s">
         <v>337</v>
       </c>
       <c r="D63" s="68" t="s">
@@ -5973,10 +6158,10 @@
     </row>
     <row r="64" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A64" s="66"/>
-      <c r="B64" s="92" t="s">
+      <c r="B64" s="82" t="s">
         <v>343</v>
       </c>
-      <c r="C64" s="92" t="s">
+      <c r="C64" s="82" t="s">
         <v>78</v>
       </c>
       <c r="D64" s="68" t="s">
@@ -6021,10 +6206,10 @@
     </row>
     <row r="65" spans="1:26" ht="106.2" thickBot="1">
       <c r="A65" s="66"/>
-      <c r="B65" s="92" t="s">
+      <c r="B65" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C65" s="92" t="s">
+      <c r="C65" s="82" t="s">
         <v>207</v>
       </c>
       <c r="D65" s="68" t="s">
@@ -6073,10 +6258,10 @@
     </row>
     <row r="66" spans="1:26" ht="53.4" thickBot="1">
       <c r="A66" s="66"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C66" s="92" t="s">
+      <c r="C66" s="82" t="s">
         <v>207</v>
       </c>
       <c r="D66" s="68" t="s">
@@ -6121,10 +6306,10 @@
     </row>
     <row r="67" spans="1:26" ht="396.6" thickBot="1">
       <c r="A67" s="66"/>
-      <c r="B67" s="92" t="s">
+      <c r="B67" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="C67" s="92" t="s">
+      <c r="C67" s="82" t="s">
         <v>274</v>
       </c>
       <c r="D67" s="68" t="s">
@@ -6173,10 +6358,10 @@
     </row>
     <row r="68" spans="1:26" ht="79.8" thickBot="1">
       <c r="A68" s="66"/>
-      <c r="B68" s="92" t="s">
+      <c r="B68" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="C68" s="92" t="s">
+      <c r="C68" s="82" t="s">
         <v>274</v>
       </c>
       <c r="D68" s="68" t="s">
@@ -6223,7 +6408,7 @@
     </row>
     <row r="69" spans="1:26" ht="132.6" thickBot="1">
       <c r="A69" s="66"/>
-      <c r="B69" s="92" t="s">
+      <c r="B69" s="82" t="s">
         <v>273</v>
       </c>
       <c r="C69" s="67" t="s">
@@ -6273,7 +6458,7 @@
     </row>
     <row r="70" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A70" s="66"/>
-      <c r="B70" s="92" t="s">
+      <c r="B70" s="82" t="s">
         <v>273</v>
       </c>
       <c r="C70" s="67" t="s">
@@ -6321,7 +6506,7 @@
     </row>
     <row r="71" spans="1:26" ht="159" thickBot="1">
       <c r="A71" s="66"/>
-      <c r="B71" s="92" t="s">
+      <c r="B71" s="82" t="s">
         <v>170</v>
       </c>
       <c r="C71" s="67" t="s">
@@ -7623,107 +7808,253 @@
       <c r="Y96" s="36"/>
       <c r="Z96" s="36"/>
     </row>
-    <row r="97" spans="1:18">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
-      <c r="K97" s="4"/>
-      <c r="L97" s="4"/>
-      <c r="M97" s="4"/>
-      <c r="N97" s="4"/>
-      <c r="O97" s="4"/>
-      <c r="P97" s="4"/>
-      <c r="Q97" s="4"/>
-      <c r="R97" s="4"/>
-    </row>
-    <row r="98" spans="1:18">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="4"/>
-      <c r="K98" s="4"/>
-      <c r="L98" s="4"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="4"/>
-      <c r="O98" s="4"/>
-      <c r="P98" s="4"/>
-      <c r="Q98" s="4"/>
-      <c r="R98" s="4"/>
-    </row>
-    <row r="99" spans="1:18">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
-      <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-    </row>
-    <row r="100" spans="1:18">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
-      <c r="L100" s="4"/>
-      <c r="M100" s="4"/>
-      <c r="N100" s="4"/>
-      <c r="O100" s="4"/>
-      <c r="P100" s="4"/>
-      <c r="Q100" s="4"/>
-      <c r="R100" s="4"/>
-    </row>
-    <row r="101" spans="1:18">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-      <c r="J101" s="4"/>
-      <c r="K101" s="4"/>
-      <c r="L101" s="4"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="4"/>
-      <c r="R101" s="4"/>
-    </row>
-    <row r="102" spans="1:18">
+    <row r="97" spans="1:26" ht="143.4" customHeight="1" thickBot="1">
+      <c r="A97" s="104">
+        <v>45637</v>
+      </c>
+      <c r="B97" s="105" t="s">
+        <v>522</v>
+      </c>
+      <c r="C97" s="61" t="s">
+        <v>523</v>
+      </c>
+      <c r="D97" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E97" s="63" t="s">
+        <v>524</v>
+      </c>
+      <c r="F97" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="G97" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="H97" s="61" t="s">
+        <v>525</v>
+      </c>
+      <c r="I97" s="61" t="s">
+        <v>526</v>
+      </c>
+      <c r="J97" s="61"/>
+      <c r="K97" s="79" t="s">
+        <v>527</v>
+      </c>
+      <c r="L97" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="M97" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="N97" s="36"/>
+      <c r="O97" s="36"/>
+      <c r="P97" s="36"/>
+      <c r="Q97" s="36"/>
+      <c r="R97" s="36"/>
+      <c r="S97" s="36"/>
+      <c r="T97" s="36"/>
+      <c r="U97" s="36"/>
+      <c r="V97" s="36"/>
+      <c r="W97" s="36"/>
+      <c r="X97" s="36"/>
+      <c r="Y97" s="36"/>
+      <c r="Z97" s="36"/>
+    </row>
+    <row r="98" spans="1:26" ht="53.4" thickBot="1">
+      <c r="A98" s="66"/>
+      <c r="B98" s="107" t="s">
+        <v>527</v>
+      </c>
+      <c r="C98" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="D98" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E98" s="69" t="s">
+        <v>529</v>
+      </c>
+      <c r="F98" s="67" t="s">
+        <v>530</v>
+      </c>
+      <c r="G98" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H98" s="67" t="s">
+        <v>531</v>
+      </c>
+      <c r="I98" s="67"/>
+      <c r="J98" s="67"/>
+      <c r="K98" s="67" t="s">
+        <v>532</v>
+      </c>
+      <c r="L98" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M98" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N98" s="36"/>
+      <c r="O98" s="36"/>
+      <c r="P98" s="36"/>
+      <c r="Q98" s="36"/>
+      <c r="R98" s="36"/>
+      <c r="S98" s="36"/>
+      <c r="T98" s="36"/>
+      <c r="U98" s="36"/>
+      <c r="V98" s="36"/>
+      <c r="W98" s="36"/>
+      <c r="X98" s="36"/>
+      <c r="Y98" s="36"/>
+      <c r="Z98" s="36"/>
+    </row>
+    <row r="99" spans="1:26" ht="146.4" customHeight="1" thickBot="1">
+      <c r="A99" s="66"/>
+      <c r="B99" s="107" t="s">
+        <v>533</v>
+      </c>
+      <c r="C99" s="67" t="s">
+        <v>534</v>
+      </c>
+      <c r="D99" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E99" s="69" t="s">
+        <v>535</v>
+      </c>
+      <c r="F99" s="67" t="s">
+        <v>536</v>
+      </c>
+      <c r="G99" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H99" s="67" t="s">
+        <v>537</v>
+      </c>
+      <c r="I99" s="67" t="s">
+        <v>538</v>
+      </c>
+      <c r="J99" s="67"/>
+      <c r="K99" s="67" t="s">
+        <v>539</v>
+      </c>
+      <c r="L99" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M99" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N99" s="36"/>
+      <c r="O99" s="36"/>
+      <c r="P99" s="36"/>
+      <c r="Q99" s="36"/>
+      <c r="R99" s="36"/>
+      <c r="S99" s="36"/>
+      <c r="T99" s="36"/>
+      <c r="U99" s="36"/>
+      <c r="V99" s="36"/>
+      <c r="W99" s="36"/>
+      <c r="X99" s="36"/>
+      <c r="Y99" s="36"/>
+      <c r="Z99" s="36"/>
+    </row>
+    <row r="100" spans="1:26" ht="132.6" thickBot="1">
+      <c r="A100" s="66"/>
+      <c r="B100" s="108" t="s">
+        <v>533</v>
+      </c>
+      <c r="C100" s="109" t="s">
+        <v>516</v>
+      </c>
+      <c r="D100" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E100" s="69" t="s">
+        <v>540</v>
+      </c>
+      <c r="F100" s="67" t="s">
+        <v>541</v>
+      </c>
+      <c r="G100" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H100" s="67" t="s">
+        <v>519</v>
+      </c>
+      <c r="I100" s="67"/>
+      <c r="J100" s="67"/>
+      <c r="K100" s="67" t="s">
+        <v>542</v>
+      </c>
+      <c r="L100" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M100" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N100" s="36"/>
+      <c r="O100" s="36"/>
+      <c r="P100" s="36"/>
+      <c r="Q100" s="36"/>
+      <c r="R100" s="36"/>
+      <c r="S100" s="36"/>
+      <c r="T100" s="36"/>
+      <c r="U100" s="36"/>
+      <c r="V100" s="36"/>
+      <c r="W100" s="36"/>
+      <c r="X100" s="36"/>
+      <c r="Y100" s="36"/>
+      <c r="Z100" s="36"/>
+    </row>
+    <row r="101" spans="1:26" ht="145.80000000000001" thickBot="1">
+      <c r="A101" s="66"/>
+      <c r="B101" s="74" t="s">
+        <v>543</v>
+      </c>
+      <c r="C101" s="67" t="s">
+        <v>544</v>
+      </c>
+      <c r="D101" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E101" s="69" t="s">
+        <v>545</v>
+      </c>
+      <c r="F101" s="67" t="s">
+        <v>546</v>
+      </c>
+      <c r="G101" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H101" s="67" t="s">
+        <v>547</v>
+      </c>
+      <c r="I101" s="67"/>
+      <c r="J101" s="67"/>
+      <c r="K101" s="67" t="s">
+        <v>548</v>
+      </c>
+      <c r="L101" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M101" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N101" s="36"/>
+      <c r="O101" s="36"/>
+      <c r="P101" s="36"/>
+      <c r="Q101" s="36"/>
+      <c r="R101" s="36"/>
+      <c r="S101" s="36"/>
+      <c r="T101" s="36"/>
+      <c r="U101" s="36"/>
+      <c r="V101" s="36"/>
+      <c r="W101" s="36"/>
+      <c r="X101" s="36"/>
+      <c r="Y101" s="36"/>
+      <c r="Z101" s="36"/>
+    </row>
+    <row r="102" spans="1:26">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -7743,7 +8074,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:26">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -7763,7 +8094,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:26">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -7783,7 +8114,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:26">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -7803,7 +8134,7 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:26">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -7823,7 +8154,7 @@
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:26">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -7843,7 +8174,7 @@
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:26">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -7863,7 +8194,7 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:26">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -7883,7 +8214,7 @@
       <c r="Q109" s="4"/>
       <c r="R109" s="4"/>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:26">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -7903,7 +8234,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:26">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -7923,7 +8254,7 @@
       <c r="Q111" s="4"/>
       <c r="R111" s="4"/>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:26">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -25765,14 +26096,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -25787,6 +26110,14 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -25846,9 +26177,15 @@
     <hyperlink ref="J95" r:id="rId47"/>
     <hyperlink ref="B96" r:id="rId48" display="https://jira.ibos.io/browse/MGM-7523"/>
     <hyperlink ref="J96" r:id="rId49"/>
+    <hyperlink ref="B97" r:id="rId50" display="https://jira.ibos.io/browse/MGM-7563"/>
+    <hyperlink ref="K97" r:id="rId51" display="https://jira.ibos.io/browse/MGM-7563"/>
+    <hyperlink ref="B98" r:id="rId52" display="https://jira.ibos.io/browse/MGM-7563"/>
+    <hyperlink ref="B99" r:id="rId53" display="https://jira.ibos.io/browse/MGM-7563"/>
+    <hyperlink ref="B100" r:id="rId54" display="https://jira.ibos.io/browse/MGM-7563"/>
+    <hyperlink ref="B101" r:id="rId55" display="https://jira.ibos.io/browse/MGM-7563"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
months wise sales and collection report
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="659">
   <si>
     <t>Product Name</t>
   </si>
@@ -2275,6 +2275,366 @@
   </si>
   <si>
     <t>It should be successfully showing include attachtment file.</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7527</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Purchase Payment</t>
+    </r>
+  </si>
+  <si>
+    <t>MGM-7609</t>
+  </si>
+  <si>
+    <t>Production Details Report</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7609</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Production </t>
+    </r>
+  </si>
+  <si>
+    <t>Create BOM</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>Try to create multiple Bom &amp; single Bom</t>
+  </si>
+  <si>
+    <t>production-Bill Of Material-Create Bill Of Material-fillup the form-save</t>
+  </si>
+  <si>
+    <t>It should be created successfully multiple Bom &amp; single Bom</t>
+  </si>
+  <si>
+    <t>Production Order</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>Try to create Production Order</t>
+  </si>
+  <si>
+    <t>production-Production Order-Create Production Order-fillup the form-save</t>
+  </si>
+  <si>
+    <t>It should be created successfully Production Order</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7609</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Approval </t>
+    </r>
+  </si>
+  <si>
+    <t>Approval Production Order</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Try to Approval Production Order</t>
+  </si>
+  <si>
+    <t>Approval-Production Order Approval-Order Approval-select-Approve-yes</t>
+  </si>
+  <si>
+    <t>It should be successfully Approve Production Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval Item Requisition
+</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>Try to Item Requisition
+Approval with Production Order</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MGM-7651
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>configuration</t>
+    </r>
+  </si>
+  <si>
+    <t>Item create</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>Try to Create Item profile with Plastics Division</t>
+  </si>
+  <si>
+    <t>configuration-add Item-AutoBarCode-select Division-select Category-fillup form-save</t>
+  </si>
+  <si>
+    <t>Master Item name-mouse onee
+Department - Plastics 
+Category- test one
+Sub Category-test two
+Minor Category-test three 
+Tag Customer-PRT-M0211 - akasaash (0179453555)</t>
+  </si>
+  <si>
+    <t>It should be successfully Create Item profile with Division</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>Try to Create Item profile with metral Division</t>
+  </si>
+  <si>
+    <t>Master Item name-cablee
+Department - metral
+Category-metral one
+Sub Category-metral two
+Minor Category-metral three 
+Tag Customer-PRT-M0211 - akasaash (0179453555)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MGM-7651
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sales Delivery 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Direct Delivery
+</t>
+  </si>
+  <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>Try to Create Direct Delivery with Plastics Division Item</t>
+  </si>
+  <si>
+    <t>Sales -Sales Delivery-Create Direct Delivery-select depetment Item- fillup form-save</t>
+  </si>
+  <si>
+    <t>Office-MGM Head Office 
+Warehouse-MGM Warehouse bd 
+Customer -555555 - Akash Dhaka (01705280423) 
+Item -mouse onee 
+Quantity -4 
+Unit Price-10</t>
+  </si>
+  <si>
+    <t>It should be successfully Create Direct Delivery</t>
+  </si>
+  <si>
+    <t>Direct Delivery</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>Try to Direct Delivery confirm</t>
+  </si>
+  <si>
+    <t>Sales -Sales Delivery-Delivery list-action -confirm</t>
+  </si>
+  <si>
+    <t>Sales -Sales Collection -due list-view-Actions-Cash Type-select Invoice-Collection amount-save</t>
+  </si>
+  <si>
+    <t>It should be successfully Direct Delivery confirm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MGM-7651
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sales Collection
+</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Try to Sales Collection in due list</t>
+  </si>
+  <si>
+    <t>Office-MGM Head Office
+Cash Type -Cash in hand
+Invoice-SD-M241200140
+Collection-50</t>
+  </si>
+  <si>
+    <t>It should be successfully due list in Sales Collection</t>
+  </si>
+  <si>
+    <t>Bill Create</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>Try to Sales Collection in Bill Create</t>
+  </si>
+  <si>
+    <t>Sales -Sales Collection -Bill Create-fillup form-select Invoice -Create Bill</t>
+  </si>
+  <si>
+    <t>Office -MGM Head Office 
+Customer -AAA (32556789899) 
+Invoice No- SD-M241200022</t>
+  </si>
+  <si>
+    <t>Collection by Invoice</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>Try to Sales Collection in Collection by Invoice</t>
+  </si>
+  <si>
+    <t>Sales -Sales Collection -Collection by Invoice-fillup form-select Customer/Invoice -save</t>
+  </si>
+  <si>
+    <t>Office-MGM Head Office 
+Cash Type-Cash in hand 
+Customer-Akashh 
+Invoice -SD-M240200037 
+Collection Amount- 22</t>
+  </si>
+  <si>
+    <t>Collected Invoice</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>Try to Sales Collection in Collected Invoice</t>
+  </si>
+  <si>
+    <t>Sales -Sales Collection -Collected Invoice -Collection Amount</t>
+  </si>
+  <si>
+    <t>Due Invoice</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>Try to Sales Collection in Due Amount with Invoice No</t>
+  </si>
+  <si>
+    <t>Sales -Sales Collection -Due Invoice-select Invoice -Due Amount</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MGM-7651
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sales Report 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Report
+</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Try to showing Month Wise Sales vs Collection Report in Sales Report
+summary and check box Sales Report details</t>
+  </si>
+  <si>
+    <t>Sales -Sales Report -select View By-View</t>
+  </si>
+  <si>
+    <t>View By-Month Wise Sales VS Collection
+Year-2024
+From Month-December
+To Month-December
+Item Category-test one
+Customer Group-All
+Customer-Akash</t>
   </si>
 </sst>
 </file>
@@ -2808,7 +3168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3073,33 +3433,36 @@
     <xf numFmtId="0" fontId="20" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3322,8 +3685,8 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O122" sqref="O122"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J122" sqref="J122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -3338,11 +3701,11 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="46"/>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="108" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="101"/>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="105" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="101"/>
@@ -3350,11 +3713,11 @@
         <v>2</v>
       </c>
       <c r="G1" s="101"/>
-      <c r="H1" s="106">
+      <c r="H1" s="109">
         <v>45615</v>
       </c>
       <c r="I1" s="101"/>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="107" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="101"/>
@@ -3370,11 +3733,11 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="46"/>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="108" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="101"/>
-      <c r="D2" s="103" t="s">
+      <c r="D2" s="105" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="101"/>
@@ -3382,14 +3745,14 @@
         <v>7</v>
       </c>
       <c r="G2" s="101"/>
-      <c r="H2" s="105"/>
+      <c r="H2" s="103"/>
       <c r="I2" s="101"/>
       <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="50">
         <f>COUNTIF(M8:M1821,"Pass")</f>
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="L2" s="51" t="s">
         <v>9</v>
@@ -3403,15 +3766,15 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="46"/>
-      <c r="B3" s="108"/>
+      <c r="B3" s="102"/>
       <c r="C3" s="101"/>
-      <c r="D3" s="105"/>
+      <c r="D3" s="103"/>
       <c r="E3" s="101"/>
       <c r="F3" s="104" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="101"/>
-      <c r="H3" s="105"/>
+      <c r="H3" s="103"/>
       <c r="I3" s="101"/>
       <c r="J3" s="52" t="s">
         <v>11</v>
@@ -3432,11 +3795,11 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="46"/>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="108" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="101"/>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="105" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="101"/>
@@ -3444,7 +3807,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="101"/>
-      <c r="H4" s="109"/>
+      <c r="H4" s="106"/>
       <c r="I4" s="101"/>
       <c r="J4" s="49" t="s">
         <v>16</v>
@@ -3465,11 +3828,11 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="46"/>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="108" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="101"/>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="105" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="101"/>
@@ -3477,7 +3840,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="101"/>
-      <c r="H5" s="105" t="s">
+      <c r="H5" s="103" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="101"/>
@@ -3486,7 +3849,7 @@
       </c>
       <c r="K5" s="57">
         <f>SUM(K2+K3+K4)</f>
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="L5" s="51" t="s">
         <v>23</v>
@@ -3501,7 +3864,7 @@
     <row r="6" spans="1:26">
       <c r="A6" s="58"/>
       <c r="B6" s="58"/>
-      <c r="C6" s="107"/>
+      <c r="C6" s="100"/>
       <c r="D6" s="101"/>
       <c r="E6" s="101"/>
       <c r="F6" s="101"/>
@@ -8567,7 +8930,7 @@
     <row r="109" spans="1:26" ht="79.8" thickBot="1">
       <c r="A109" s="66"/>
       <c r="B109" s="74" t="s">
-        <v>565</v>
+        <v>583</v>
       </c>
       <c r="C109" s="67" t="s">
         <v>578</v>
@@ -8612,307 +8975,723 @@
       <c r="Y109" s="36"/>
       <c r="Z109" s="36"/>
     </row>
-    <row r="110" spans="1:26">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
-      <c r="K110" s="4"/>
-      <c r="L110" s="4"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="4"/>
-      <c r="O110" s="4"/>
-      <c r="P110" s="4"/>
-      <c r="Q110" s="4"/>
-      <c r="R110" s="4"/>
-    </row>
-    <row r="111" spans="1:26">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="4"/>
-      <c r="J111" s="4"/>
-      <c r="K111" s="4"/>
-      <c r="L111" s="4"/>
-      <c r="M111" s="4"/>
-      <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
-      <c r="Q111" s="4"/>
-      <c r="R111" s="4"/>
-    </row>
-    <row r="112" spans="1:26">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="4"/>
-      <c r="K112" s="4"/>
-      <c r="L112" s="4"/>
-      <c r="M112" s="4"/>
-      <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
-      <c r="Q112" s="4"/>
-      <c r="R112" s="4"/>
-    </row>
-    <row r="113" spans="1:18">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="4"/>
-      <c r="K113" s="4"/>
-      <c r="L113" s="4"/>
-      <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="Q113" s="4"/>
-      <c r="R113" s="4"/>
-    </row>
-    <row r="114" spans="1:18">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-      <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
-      <c r="J114" s="4"/>
-      <c r="K114" s="4"/>
-      <c r="L114" s="4"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
-      <c r="Q114" s="4"/>
-      <c r="R114" s="4"/>
-    </row>
-    <row r="115" spans="1:18">
-      <c r="A115" s="4"/>
-      <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
-      <c r="E115" s="4"/>
-      <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
-      <c r="J115" s="4"/>
-      <c r="K115" s="4"/>
-      <c r="L115" s="4"/>
-      <c r="M115" s="4"/>
-      <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
-      <c r="Q115" s="4"/>
-      <c r="R115" s="4"/>
-    </row>
-    <row r="116" spans="1:18">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
-      <c r="G116" s="4"/>
-      <c r="H116" s="4"/>
-      <c r="I116" s="4"/>
-      <c r="J116" s="4"/>
-      <c r="K116" s="4"/>
-      <c r="L116" s="4"/>
-      <c r="M116" s="4"/>
-      <c r="N116" s="4"/>
-      <c r="O116" s="4"/>
-      <c r="P116" s="4"/>
-      <c r="Q116" s="4"/>
-      <c r="R116" s="4"/>
-    </row>
-    <row r="117" spans="1:18">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
-      <c r="J117" s="4"/>
-      <c r="K117" s="4"/>
-      <c r="L117" s="4"/>
-      <c r="M117" s="4"/>
-      <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
-      <c r="Q117" s="4"/>
-      <c r="R117" s="4"/>
-    </row>
-    <row r="118" spans="1:18">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="4"/>
-      <c r="G118" s="4"/>
-      <c r="H118" s="4"/>
-      <c r="I118" s="4"/>
-      <c r="J118" s="4"/>
-      <c r="K118" s="4"/>
-      <c r="L118" s="4"/>
-      <c r="M118" s="4"/>
-      <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
-      <c r="Q118" s="4"/>
-      <c r="R118" s="4"/>
-    </row>
-    <row r="119" spans="1:18">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="4"/>
-      <c r="H119" s="4"/>
-      <c r="I119" s="4"/>
-      <c r="J119" s="4"/>
-      <c r="K119" s="4"/>
-      <c r="L119" s="4"/>
-      <c r="M119" s="4"/>
-      <c r="N119" s="4"/>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
-      <c r="Q119" s="4"/>
-      <c r="R119" s="4"/>
-    </row>
-    <row r="120" spans="1:18">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
-      <c r="J120" s="4"/>
-      <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-    </row>
-    <row r="121" spans="1:18">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="4"/>
-      <c r="J121" s="4"/>
-      <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-      <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-    </row>
-    <row r="122" spans="1:18">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
-      <c r="I122" s="4"/>
-      <c r="J122" s="4"/>
-      <c r="K122" s="4"/>
-      <c r="L122" s="4"/>
-      <c r="M122" s="4"/>
-      <c r="N122" s="4"/>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
-      <c r="Q122" s="4"/>
-      <c r="R122" s="4"/>
-    </row>
-    <row r="123" spans="1:18">
-      <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
-      <c r="I123" s="4"/>
-      <c r="J123" s="4"/>
-      <c r="K123" s="4"/>
-      <c r="L123" s="4"/>
-      <c r="M123" s="4"/>
-      <c r="N123" s="4"/>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
-      <c r="Q123" s="4"/>
-      <c r="R123" s="4"/>
-    </row>
-    <row r="124" spans="1:18">
-      <c r="A124" s="4"/>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="4"/>
-      <c r="I124" s="4"/>
-      <c r="J124" s="4"/>
-      <c r="K124" s="4"/>
-      <c r="L124" s="4"/>
-      <c r="M124" s="4"/>
-      <c r="N124" s="4"/>
-      <c r="O124" s="4"/>
-      <c r="P124" s="4"/>
-      <c r="Q124" s="4"/>
-      <c r="R124" s="4"/>
-    </row>
-    <row r="125" spans="1:18">
+    <row r="110" spans="1:26" ht="27" thickBot="1">
+      <c r="A110" s="94">
+        <v>45638</v>
+      </c>
+      <c r="B110" s="110" t="s">
+        <v>584</v>
+      </c>
+      <c r="C110" s="61" t="s">
+        <v>585</v>
+      </c>
+      <c r="D110" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E110" s="63" t="s">
+        <v>586</v>
+      </c>
+      <c r="F110" s="61"/>
+      <c r="G110" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="H110" s="61"/>
+      <c r="I110" s="61"/>
+      <c r="J110" s="61"/>
+      <c r="K110" s="61"/>
+      <c r="L110" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="M110" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="N110" s="36"/>
+      <c r="O110" s="36"/>
+      <c r="P110" s="36"/>
+      <c r="Q110" s="36"/>
+      <c r="R110" s="36"/>
+      <c r="S110" s="36"/>
+      <c r="T110" s="36"/>
+      <c r="U110" s="36"/>
+      <c r="V110" s="36"/>
+      <c r="W110" s="36"/>
+      <c r="X110" s="36"/>
+      <c r="Y110" s="36"/>
+      <c r="Z110" s="36"/>
+    </row>
+    <row r="111" spans="1:26" ht="66.599999999999994" thickBot="1">
+      <c r="A111" s="66"/>
+      <c r="B111" s="74" t="s">
+        <v>587</v>
+      </c>
+      <c r="C111" s="67" t="s">
+        <v>588</v>
+      </c>
+      <c r="D111" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E111" s="69" t="s">
+        <v>589</v>
+      </c>
+      <c r="F111" s="67" t="s">
+        <v>590</v>
+      </c>
+      <c r="G111" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H111" s="67" t="s">
+        <v>591</v>
+      </c>
+      <c r="I111" s="67"/>
+      <c r="J111" s="67"/>
+      <c r="K111" s="67" t="s">
+        <v>592</v>
+      </c>
+      <c r="L111" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M111" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N111" s="36"/>
+      <c r="O111" s="36"/>
+      <c r="P111" s="36"/>
+      <c r="Q111" s="36"/>
+      <c r="R111" s="36"/>
+      <c r="S111" s="36"/>
+      <c r="T111" s="36"/>
+      <c r="U111" s="36"/>
+      <c r="V111" s="36"/>
+      <c r="W111" s="36"/>
+      <c r="X111" s="36"/>
+      <c r="Y111" s="36"/>
+      <c r="Z111" s="36"/>
+    </row>
+    <row r="112" spans="1:26" ht="66.599999999999994" thickBot="1">
+      <c r="A112" s="66"/>
+      <c r="B112" s="74" t="s">
+        <v>587</v>
+      </c>
+      <c r="C112" s="67" t="s">
+        <v>593</v>
+      </c>
+      <c r="D112" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E112" s="69" t="s">
+        <v>594</v>
+      </c>
+      <c r="F112" s="67" t="s">
+        <v>595</v>
+      </c>
+      <c r="G112" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H112" s="67" t="s">
+        <v>596</v>
+      </c>
+      <c r="I112" s="67"/>
+      <c r="J112" s="67"/>
+      <c r="K112" s="67" t="s">
+        <v>597</v>
+      </c>
+      <c r="L112" s="71"/>
+      <c r="M112" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N112" s="36"/>
+      <c r="O112" s="36"/>
+      <c r="P112" s="36"/>
+      <c r="Q112" s="36"/>
+      <c r="R112" s="36"/>
+      <c r="S112" s="36"/>
+      <c r="T112" s="36"/>
+      <c r="U112" s="36"/>
+      <c r="V112" s="36"/>
+      <c r="W112" s="36"/>
+      <c r="X112" s="36"/>
+      <c r="Y112" s="36"/>
+      <c r="Z112" s="36"/>
+    </row>
+    <row r="113" spans="1:26" ht="66.599999999999994" thickBot="1">
+      <c r="A113" s="66"/>
+      <c r="B113" s="74" t="s">
+        <v>598</v>
+      </c>
+      <c r="C113" s="67" t="s">
+        <v>599</v>
+      </c>
+      <c r="D113" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E113" s="69" t="s">
+        <v>600</v>
+      </c>
+      <c r="F113" s="67" t="s">
+        <v>601</v>
+      </c>
+      <c r="G113" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H113" s="67" t="s">
+        <v>602</v>
+      </c>
+      <c r="I113" s="67"/>
+      <c r="J113" s="67"/>
+      <c r="K113" s="67" t="s">
+        <v>603</v>
+      </c>
+      <c r="L113" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M113" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N113" s="36"/>
+      <c r="O113" s="36"/>
+      <c r="P113" s="36"/>
+      <c r="Q113" s="36"/>
+      <c r="R113" s="36"/>
+      <c r="S113" s="36"/>
+      <c r="T113" s="36"/>
+      <c r="U113" s="36"/>
+      <c r="V113" s="36"/>
+      <c r="W113" s="36"/>
+      <c r="X113" s="36"/>
+      <c r="Y113" s="36"/>
+      <c r="Z113" s="36"/>
+    </row>
+    <row r="114" spans="1:26" ht="53.4" thickBot="1">
+      <c r="A114" s="66"/>
+      <c r="B114" s="74" t="s">
+        <v>598</v>
+      </c>
+      <c r="C114" s="67" t="s">
+        <v>604</v>
+      </c>
+      <c r="D114" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E114" s="69" t="s">
+        <v>605</v>
+      </c>
+      <c r="F114" s="67" t="s">
+        <v>606</v>
+      </c>
+      <c r="G114" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H114" s="67"/>
+      <c r="I114" s="67"/>
+      <c r="J114" s="67"/>
+      <c r="K114" s="67"/>
+      <c r="L114" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M114" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N114" s="36"/>
+      <c r="O114" s="36"/>
+      <c r="P114" s="36"/>
+      <c r="Q114" s="36"/>
+      <c r="R114" s="36"/>
+      <c r="S114" s="36"/>
+      <c r="T114" s="36"/>
+      <c r="U114" s="36"/>
+      <c r="V114" s="36"/>
+      <c r="W114" s="36"/>
+      <c r="X114" s="36"/>
+      <c r="Y114" s="36"/>
+      <c r="Z114" s="36"/>
+    </row>
+    <row r="115" spans="1:26" ht="211.8" thickBot="1">
+      <c r="A115" s="73">
+        <v>45643</v>
+      </c>
+      <c r="B115" s="74" t="s">
+        <v>607</v>
+      </c>
+      <c r="C115" s="67" t="s">
+        <v>608</v>
+      </c>
+      <c r="D115" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E115" s="69" t="s">
+        <v>609</v>
+      </c>
+      <c r="F115" s="67" t="s">
+        <v>610</v>
+      </c>
+      <c r="G115" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H115" s="67" t="s">
+        <v>611</v>
+      </c>
+      <c r="I115" s="71"/>
+      <c r="J115" s="67" t="s">
+        <v>612</v>
+      </c>
+      <c r="K115" s="67" t="s">
+        <v>613</v>
+      </c>
+      <c r="L115" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M115" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N115" s="36"/>
+      <c r="O115" s="36"/>
+      <c r="P115" s="36"/>
+      <c r="Q115" s="36"/>
+      <c r="R115" s="36"/>
+      <c r="S115" s="36"/>
+      <c r="T115" s="36"/>
+      <c r="U115" s="36"/>
+      <c r="V115" s="36"/>
+      <c r="W115" s="36"/>
+      <c r="X115" s="36"/>
+      <c r="Y115" s="36"/>
+      <c r="Z115" s="36"/>
+    </row>
+    <row r="116" spans="1:26" ht="198.6" thickBot="1">
+      <c r="A116" s="66"/>
+      <c r="B116" s="74" t="s">
+        <v>607</v>
+      </c>
+      <c r="C116" s="67" t="s">
+        <v>608</v>
+      </c>
+      <c r="D116" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E116" s="69" t="s">
+        <v>614</v>
+      </c>
+      <c r="F116" s="67" t="s">
+        <v>615</v>
+      </c>
+      <c r="G116" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H116" s="67" t="s">
+        <v>611</v>
+      </c>
+      <c r="I116" s="67"/>
+      <c r="J116" s="67" t="s">
+        <v>616</v>
+      </c>
+      <c r="K116" s="67" t="s">
+        <v>613</v>
+      </c>
+      <c r="L116" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M116" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N116" s="36"/>
+      <c r="O116" s="36"/>
+      <c r="P116" s="36"/>
+      <c r="Q116" s="36"/>
+      <c r="R116" s="36"/>
+      <c r="S116" s="36"/>
+      <c r="T116" s="36"/>
+      <c r="U116" s="36"/>
+      <c r="V116" s="36"/>
+      <c r="W116" s="36"/>
+      <c r="X116" s="36"/>
+      <c r="Y116" s="36"/>
+      <c r="Z116" s="36"/>
+    </row>
+    <row r="117" spans="1:26" ht="198.6" thickBot="1">
+      <c r="A117" s="66"/>
+      <c r="B117" s="74" t="s">
+        <v>617</v>
+      </c>
+      <c r="C117" s="67" t="s">
+        <v>618</v>
+      </c>
+      <c r="D117" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E117" s="69" t="s">
+        <v>619</v>
+      </c>
+      <c r="F117" s="67" t="s">
+        <v>620</v>
+      </c>
+      <c r="G117" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H117" s="67" t="s">
+        <v>621</v>
+      </c>
+      <c r="I117" s="67"/>
+      <c r="J117" s="67" t="s">
+        <v>622</v>
+      </c>
+      <c r="K117" s="67" t="s">
+        <v>623</v>
+      </c>
+      <c r="L117" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M117" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N117" s="36"/>
+      <c r="O117" s="36"/>
+      <c r="P117" s="36"/>
+      <c r="Q117" s="36"/>
+      <c r="R117" s="36"/>
+      <c r="S117" s="36"/>
+      <c r="T117" s="36"/>
+      <c r="U117" s="36"/>
+      <c r="V117" s="36"/>
+      <c r="W117" s="36"/>
+      <c r="X117" s="36"/>
+      <c r="Y117" s="36"/>
+      <c r="Z117" s="36"/>
+    </row>
+    <row r="118" spans="1:26" ht="106.2" thickBot="1">
+      <c r="A118" s="66"/>
+      <c r="B118" s="74" t="s">
+        <v>617</v>
+      </c>
+      <c r="C118" s="67" t="s">
+        <v>624</v>
+      </c>
+      <c r="D118" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E118" s="69" t="s">
+        <v>625</v>
+      </c>
+      <c r="F118" s="67" t="s">
+        <v>626</v>
+      </c>
+      <c r="G118" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H118" s="67" t="s">
+        <v>627</v>
+      </c>
+      <c r="I118" s="67"/>
+      <c r="J118" s="67" t="s">
+        <v>628</v>
+      </c>
+      <c r="K118" s="67" t="s">
+        <v>629</v>
+      </c>
+      <c r="L118" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M118" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N118" s="36"/>
+      <c r="O118" s="36"/>
+      <c r="P118" s="36"/>
+      <c r="Q118" s="36"/>
+      <c r="R118" s="36"/>
+      <c r="S118" s="36"/>
+      <c r="T118" s="36"/>
+      <c r="U118" s="36"/>
+      <c r="V118" s="36"/>
+      <c r="W118" s="36"/>
+      <c r="X118" s="36"/>
+      <c r="Y118" s="36"/>
+      <c r="Z118" s="36"/>
+    </row>
+    <row r="119" spans="1:26" ht="93" thickBot="1">
+      <c r="A119" s="66"/>
+      <c r="B119" s="74" t="s">
+        <v>630</v>
+      </c>
+      <c r="C119" s="67" t="s">
+        <v>566</v>
+      </c>
+      <c r="D119" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E119" s="69" t="s">
+        <v>631</v>
+      </c>
+      <c r="F119" s="67" t="s">
+        <v>632</v>
+      </c>
+      <c r="G119" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H119" s="67" t="s">
+        <v>628</v>
+      </c>
+      <c r="I119" s="67"/>
+      <c r="J119" s="67" t="s">
+        <v>633</v>
+      </c>
+      <c r="K119" s="67" t="s">
+        <v>634</v>
+      </c>
+      <c r="L119" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M119" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N119" s="36"/>
+      <c r="O119" s="36"/>
+      <c r="P119" s="36"/>
+      <c r="Q119" s="36"/>
+      <c r="R119" s="36"/>
+      <c r="S119" s="36"/>
+      <c r="T119" s="36"/>
+      <c r="U119" s="36"/>
+      <c r="V119" s="36"/>
+      <c r="W119" s="36"/>
+      <c r="X119" s="36"/>
+      <c r="Y119" s="36"/>
+      <c r="Z119" s="36"/>
+    </row>
+    <row r="120" spans="1:26" ht="119.4" thickBot="1">
+      <c r="A120" s="66"/>
+      <c r="B120" s="74" t="s">
+        <v>630</v>
+      </c>
+      <c r="C120" s="67" t="s">
+        <v>635</v>
+      </c>
+      <c r="D120" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E120" s="69" t="s">
+        <v>636</v>
+      </c>
+      <c r="F120" s="67" t="s">
+        <v>637</v>
+      </c>
+      <c r="G120" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H120" s="67" t="s">
+        <v>638</v>
+      </c>
+      <c r="I120" s="67"/>
+      <c r="J120" s="67" t="s">
+        <v>639</v>
+      </c>
+      <c r="K120" s="67"/>
+      <c r="L120" s="71"/>
+      <c r="M120" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N120" s="36"/>
+      <c r="O120" s="36"/>
+      <c r="P120" s="36"/>
+      <c r="Q120" s="36"/>
+      <c r="R120" s="36"/>
+      <c r="S120" s="36"/>
+      <c r="T120" s="36"/>
+      <c r="U120" s="36"/>
+      <c r="V120" s="36"/>
+      <c r="W120" s="36"/>
+      <c r="X120" s="36"/>
+      <c r="Y120" s="36"/>
+      <c r="Z120" s="36"/>
+    </row>
+    <row r="121" spans="1:26" ht="132.6" thickBot="1">
+      <c r="A121" s="66"/>
+      <c r="B121" s="74" t="s">
+        <v>630</v>
+      </c>
+      <c r="C121" s="67" t="s">
+        <v>640</v>
+      </c>
+      <c r="D121" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E121" s="69" t="s">
+        <v>641</v>
+      </c>
+      <c r="F121" s="67" t="s">
+        <v>642</v>
+      </c>
+      <c r="G121" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H121" s="67" t="s">
+        <v>643</v>
+      </c>
+      <c r="I121" s="67"/>
+      <c r="J121" s="67" t="s">
+        <v>644</v>
+      </c>
+      <c r="K121" s="67"/>
+      <c r="L121" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M121" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N121" s="36"/>
+      <c r="O121" s="36"/>
+      <c r="P121" s="36"/>
+      <c r="Q121" s="36"/>
+      <c r="R121" s="36"/>
+      <c r="S121" s="36"/>
+      <c r="T121" s="36"/>
+      <c r="U121" s="36"/>
+      <c r="V121" s="36"/>
+      <c r="W121" s="36"/>
+      <c r="X121" s="36"/>
+      <c r="Y121" s="36"/>
+      <c r="Z121" s="36"/>
+    </row>
+    <row r="122" spans="1:26" ht="66.599999999999994" thickBot="1">
+      <c r="A122" s="66"/>
+      <c r="B122" s="74" t="s">
+        <v>630</v>
+      </c>
+      <c r="C122" s="67" t="s">
+        <v>645</v>
+      </c>
+      <c r="D122" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E122" s="69" t="s">
+        <v>646</v>
+      </c>
+      <c r="F122" s="67" t="s">
+        <v>647</v>
+      </c>
+      <c r="G122" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H122" s="67" t="s">
+        <v>648</v>
+      </c>
+      <c r="I122" s="67"/>
+      <c r="J122" s="67"/>
+      <c r="K122" s="67"/>
+      <c r="L122" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M122" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N122" s="36"/>
+      <c r="O122" s="36"/>
+      <c r="P122" s="36"/>
+      <c r="Q122" s="36"/>
+      <c r="R122" s="36"/>
+      <c r="S122" s="36"/>
+      <c r="T122" s="36"/>
+      <c r="U122" s="36"/>
+      <c r="V122" s="36"/>
+      <c r="W122" s="36"/>
+      <c r="X122" s="36"/>
+      <c r="Y122" s="36"/>
+      <c r="Z122" s="36"/>
+    </row>
+    <row r="123" spans="1:26" ht="66.599999999999994" thickBot="1">
+      <c r="A123" s="66"/>
+      <c r="B123" s="74" t="s">
+        <v>630</v>
+      </c>
+      <c r="C123" s="67" t="s">
+        <v>649</v>
+      </c>
+      <c r="D123" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E123" s="69" t="s">
+        <v>650</v>
+      </c>
+      <c r="F123" s="67" t="s">
+        <v>651</v>
+      </c>
+      <c r="G123" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H123" s="67" t="s">
+        <v>652</v>
+      </c>
+      <c r="I123" s="67"/>
+      <c r="J123" s="67"/>
+      <c r="K123" s="67"/>
+      <c r="L123" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M123" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N123" s="36"/>
+      <c r="O123" s="36"/>
+      <c r="P123" s="36"/>
+      <c r="Q123" s="36"/>
+      <c r="R123" s="36"/>
+      <c r="S123" s="36"/>
+      <c r="T123" s="36"/>
+      <c r="U123" s="36"/>
+      <c r="V123" s="36"/>
+      <c r="W123" s="36"/>
+      <c r="X123" s="36"/>
+      <c r="Y123" s="36"/>
+      <c r="Z123" s="36"/>
+    </row>
+    <row r="124" spans="1:26" ht="198.6" thickBot="1">
+      <c r="A124" s="66"/>
+      <c r="B124" s="74" t="s">
+        <v>653</v>
+      </c>
+      <c r="C124" s="67" t="s">
+        <v>654</v>
+      </c>
+      <c r="D124" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E124" s="69" t="s">
+        <v>655</v>
+      </c>
+      <c r="F124" s="67" t="s">
+        <v>656</v>
+      </c>
+      <c r="G124" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H124" s="67" t="s">
+        <v>657</v>
+      </c>
+      <c r="I124" s="67"/>
+      <c r="J124" s="67" t="s">
+        <v>658</v>
+      </c>
+      <c r="K124" s="67"/>
+      <c r="L124" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M124" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N124" s="36"/>
+      <c r="O124" s="36"/>
+      <c r="P124" s="36"/>
+      <c r="Q124" s="36"/>
+      <c r="R124" s="36"/>
+      <c r="S124" s="36"/>
+      <c r="T124" s="36"/>
+      <c r="U124" s="36"/>
+      <c r="V124" s="36"/>
+      <c r="W124" s="36"/>
+      <c r="X124" s="36"/>
+      <c r="Y124" s="36"/>
+      <c r="Z124" s="36"/>
+    </row>
+    <row r="125" spans="1:26">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -8932,7 +9711,7 @@
       <c r="Q125" s="4"/>
       <c r="R125" s="4"/>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:26">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -8952,7 +9731,7 @@
       <c r="Q126" s="4"/>
       <c r="R126" s="4"/>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:26">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -8972,7 +9751,7 @@
       <c r="Q127" s="4"/>
       <c r="R127" s="4"/>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:26">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -26494,14 +27273,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -26516,6 +27287,14 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -26589,9 +27368,24 @@
     <hyperlink ref="B107" r:id="rId61" display="https://jira.ibos.io/browse/MGM-7527"/>
     <hyperlink ref="B108" r:id="rId62" display="https://jira.ibos.io/browse/MGM-7527"/>
     <hyperlink ref="B109" r:id="rId63" display="https://jira.ibos.io/browse/MGM-7527"/>
+    <hyperlink ref="B110" r:id="rId64" display="https://jira.ibos.io/browse/MGM-7609"/>
+    <hyperlink ref="B111" r:id="rId65" display="https://jira.ibos.io/browse/MGM-7609"/>
+    <hyperlink ref="B112" r:id="rId66" display="https://jira.ibos.io/browse/MGM-7609"/>
+    <hyperlink ref="B113" r:id="rId67" display="https://jira.ibos.io/browse/MGM-7609"/>
+    <hyperlink ref="B114" r:id="rId68" display="https://jira.ibos.io/browse/MGM-7609"/>
+    <hyperlink ref="B115" r:id="rId69" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B116" r:id="rId70" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B117" r:id="rId71" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B118" r:id="rId72" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B119" r:id="rId73" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B120" r:id="rId74" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B121" r:id="rId75" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B122" r:id="rId76" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B123" r:id="rId77" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B124" r:id="rId78" display="https://jira.ibos.io/browse/MGM-7651"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId64"/>
+  <pageSetup orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sales reports QTY sales and purchase unassigned
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="667">
   <si>
     <t>Product Name</t>
   </si>
@@ -2635,6 +2635,38 @@
 Item Category-test one
 Customer Group-All
 Customer-Akash</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Try to Month Wise Sales vs Collection Report in Sales Report
+summary without (Item Category, Customer Group Customer)Sales Report details</t>
+  </si>
+  <si>
+    <t>Sales -Sales Report -select View By- without check box-View</t>
+  </si>
+  <si>
+    <t>View By-Month Wise Sales VS Collection
+Year-2024
+From Month-December
+To Month-December
+Item Category-
+Customer Group-
+Customer-</t>
+  </si>
+  <si>
+    <t>it should showing with Unassigned issue and division together month wise sales report</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Try to Month Wise Sales vs Collection Report in
+summary Unassigned issue showing non-division item</t>
+  </si>
+  <si>
+    <t>it should be showing non-division item Unassigned issue with month wise sales report</t>
   </si>
 </sst>
 </file>
@@ -3168,7 +3200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3433,36 +3465,39 @@
     <xf numFmtId="0" fontId="20" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3685,8 +3720,8 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O123" sqref="O123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -3701,26 +3736,26 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="46"/>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="101"/>
-      <c r="D1" s="105" t="s">
+      <c r="C1" s="102"/>
+      <c r="D1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="101"/>
-      <c r="F1" s="104" t="s">
+      <c r="E1" s="102"/>
+      <c r="F1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="101"/>
-      <c r="H1" s="109">
+      <c r="G1" s="102"/>
+      <c r="H1" s="107">
         <v>45615</v>
       </c>
-      <c r="I1" s="101"/>
-      <c r="J1" s="107" t="s">
+      <c r="I1" s="102"/>
+      <c r="J1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="101"/>
+      <c r="K1" s="102"/>
       <c r="L1" s="47"/>
       <c r="M1" s="48" t="s">
         <v>4</v>
@@ -3733,26 +3768,26 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="46"/>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="105" t="s">
+      <c r="C2" s="102"/>
+      <c r="D2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="104" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="101"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="102"/>
       <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="50">
         <f>COUNTIF(M8:M1821,"Pass")</f>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L2" s="51" t="s">
         <v>9</v>
@@ -3766,16 +3801,16 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="46"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="104" t="s">
+      <c r="B3" s="109"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="101"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="102"/>
       <c r="J3" s="52" t="s">
         <v>11</v>
       </c>
@@ -3795,20 +3830,20 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="46"/>
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="105" t="s">
+      <c r="C4" s="102"/>
+      <c r="D4" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="101"/>
-      <c r="F4" s="104" t="s">
+      <c r="E4" s="102"/>
+      <c r="F4" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="101"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="101"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="102"/>
       <c r="J4" s="49" t="s">
         <v>16</v>
       </c>
@@ -3828,28 +3863,28 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="46"/>
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="105" t="s">
+      <c r="C5" s="102"/>
+      <c r="D5" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="101"/>
-      <c r="F5" s="104" t="s">
+      <c r="E5" s="102"/>
+      <c r="F5" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="101"/>
-      <c r="H5" s="103" t="s">
+      <c r="G5" s="102"/>
+      <c r="H5" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="101"/>
+      <c r="I5" s="102"/>
       <c r="J5" s="56" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="57">
         <f>SUM(K2+K3+K4)</f>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L5" s="51" t="s">
         <v>23</v>
@@ -3864,14 +3899,14 @@
     <row r="6" spans="1:26">
       <c r="A6" s="58"/>
       <c r="B6" s="58"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
       <c r="K6" s="58"/>
       <c r="L6" s="51" t="s">
         <v>24</v>
@@ -8979,7 +9014,7 @@
       <c r="A110" s="94">
         <v>45638</v>
       </c>
-      <c r="B110" s="110" t="s">
+      <c r="B110" s="100" t="s">
         <v>584</v>
       </c>
       <c r="C110" s="61" t="s">
@@ -9691,45 +9726,105 @@
       <c r="Y124" s="36"/>
       <c r="Z124" s="36"/>
     </row>
-    <row r="125" spans="1:26">
-      <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4"/>
-      <c r="E125" s="4"/>
-      <c r="F125" s="4"/>
-      <c r="G125" s="4"/>
-      <c r="H125" s="4"/>
-      <c r="I125" s="4"/>
-      <c r="J125" s="4"/>
-      <c r="K125" s="4"/>
-      <c r="L125" s="4"/>
-      <c r="M125" s="4"/>
-      <c r="N125" s="4"/>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
-      <c r="Q125" s="4"/>
-      <c r="R125" s="4"/>
-    </row>
-    <row r="126" spans="1:26">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
-      <c r="G126" s="4"/>
-      <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
-      <c r="J126" s="4"/>
-      <c r="K126" s="4"/>
-      <c r="L126" s="4"/>
-      <c r="M126" s="4"/>
-      <c r="N126" s="4"/>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
-      <c r="Q126" s="4"/>
-      <c r="R126" s="4"/>
+    <row r="125" spans="1:26" ht="172.2" thickBot="1">
+      <c r="A125" s="111"/>
+      <c r="B125" s="100" t="s">
+        <v>653</v>
+      </c>
+      <c r="C125" s="61" t="s">
+        <v>654</v>
+      </c>
+      <c r="D125" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E125" s="63" t="s">
+        <v>659</v>
+      </c>
+      <c r="F125" s="61" t="s">
+        <v>660</v>
+      </c>
+      <c r="G125" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="H125" s="61" t="s">
+        <v>661</v>
+      </c>
+      <c r="I125" s="61"/>
+      <c r="J125" s="61" t="s">
+        <v>662</v>
+      </c>
+      <c r="K125" s="61" t="s">
+        <v>663</v>
+      </c>
+      <c r="L125" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="M125" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="N125" s="36"/>
+      <c r="O125" s="36"/>
+      <c r="P125" s="36"/>
+      <c r="Q125" s="36"/>
+      <c r="R125" s="36"/>
+      <c r="S125" s="36"/>
+      <c r="T125" s="36"/>
+      <c r="U125" s="36"/>
+      <c r="V125" s="36"/>
+      <c r="W125" s="36"/>
+      <c r="X125" s="36"/>
+      <c r="Y125" s="36"/>
+      <c r="Z125" s="36"/>
+    </row>
+    <row r="126" spans="1:26" ht="172.2" thickBot="1">
+      <c r="A126" s="66"/>
+      <c r="B126" s="74" t="s">
+        <v>653</v>
+      </c>
+      <c r="C126" s="67" t="s">
+        <v>654</v>
+      </c>
+      <c r="D126" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E126" s="69" t="s">
+        <v>664</v>
+      </c>
+      <c r="F126" s="67" t="s">
+        <v>665</v>
+      </c>
+      <c r="G126" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H126" s="67" t="s">
+        <v>661</v>
+      </c>
+      <c r="I126" s="67"/>
+      <c r="J126" s="67" t="s">
+        <v>662</v>
+      </c>
+      <c r="K126" s="67" t="s">
+        <v>666</v>
+      </c>
+      <c r="L126" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M126" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N126" s="36"/>
+      <c r="O126" s="36"/>
+      <c r="P126" s="36"/>
+      <c r="Q126" s="36"/>
+      <c r="R126" s="36"/>
+      <c r="S126" s="36"/>
+      <c r="T126" s="36"/>
+      <c r="U126" s="36"/>
+      <c r="V126" s="36"/>
+      <c r="W126" s="36"/>
+      <c r="X126" s="36"/>
+      <c r="Y126" s="36"/>
+      <c r="Z126" s="36"/>
     </row>
     <row r="127" spans="1:26">
       <c r="A127" s="4"/>
@@ -27273,6 +27368,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -27287,14 +27390,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -27383,9 +27478,11 @@
     <hyperlink ref="B122" r:id="rId76" display="https://jira.ibos.io/browse/MGM-7651"/>
     <hyperlink ref="B123" r:id="rId77" display="https://jira.ibos.io/browse/MGM-7651"/>
     <hyperlink ref="B124" r:id="rId78" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B125" r:id="rId79" display="https://jira.ibos.io/browse/MGM-7651"/>
+    <hyperlink ref="B126" r:id="rId80" display="https://jira.ibos.io/browse/MGM-7651"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId79"/>
+  <pageSetup orientation="portrait" r:id="rId81"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Total Quantity in Product Request PDF
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="745">
   <si>
     <t>Product Name</t>
   </si>
@@ -2949,6 +2949,69 @@
   <si>
     <t xml:space="preserve">it will should be after Item Issue Projects Details Inventory Details Actual Qty vaild effect 
 </t>
+  </si>
+  <si>
+    <t>Create Transfer Request</t>
+  </si>
+  <si>
+    <t>Try to Create Transfer Request</t>
+  </si>
+  <si>
+    <t>Inventory -Transfer Request-Create Transfer Request-fillup form-save</t>
+  </si>
+  <si>
+    <t>Item Name Quantity 
+Wrapper 2 
+WE01 1</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/TN2Y6SXJvs60</t>
+  </si>
+  <si>
+    <t>It will should be successfully Create Transfer Request</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7873</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Transfer Request Approval</t>
+    </r>
+  </si>
+  <si>
+    <t>Inventory Approval</t>
+  </si>
+  <si>
+    <t>Try to Transfer Request Approval</t>
+  </si>
+  <si>
+    <t>Approval-Inventory Approval-Transfer Request Approval-Approve Request-Approve-yes</t>
+  </si>
+  <si>
+    <t>It will should be successfully Transfer Request Approval-</t>
+  </si>
+  <si>
+    <t>Transfer Request</t>
+  </si>
+  <si>
+    <t>Try to checking Add Total Quantity in Product Request PDF</t>
+  </si>
+  <si>
+    <t>Inventory -Transfer Request-Action- view Pdf</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/usOLjaSbZ-RI</t>
+  </si>
+  <si>
+    <t>It will should be showing Add Total Quantity in Product Request PDF</t>
   </si>
 </sst>
 </file>
@@ -3753,34 +3816,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3795,6 +3830,34 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4015,10 +4078,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P137" sqref="P137"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K159" sqref="K159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -4033,26 +4096,26 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="46"/>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="D1" s="107" t="s">
+      <c r="C1" s="108"/>
+      <c r="D1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="103"/>
-      <c r="F1" s="106" t="s">
+      <c r="E1" s="108"/>
+      <c r="F1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="103"/>
-      <c r="H1" s="111">
+      <c r="G1" s="108"/>
+      <c r="H1" s="113">
         <v>45615</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="109" t="s">
+      <c r="I1" s="108"/>
+      <c r="J1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="103"/>
+      <c r="K1" s="108"/>
       <c r="L1" s="47"/>
       <c r="M1" s="48" t="s">
         <v>4</v>
@@ -4065,26 +4128,26 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="46"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="107" t="s">
+      <c r="C2" s="108"/>
+      <c r="D2" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="103"/>
-      <c r="F2" s="106" t="s">
+      <c r="E2" s="108"/>
+      <c r="F2" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="103"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="103"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="108"/>
       <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="50">
-        <f>COUNTIF(M8:M1821,"Pass")</f>
-        <v>130</v>
+        <f>COUNTIF(M8:M1823,"Pass")</f>
+        <v>132</v>
       </c>
       <c r="L2" s="51" t="s">
         <v>9</v>
@@ -4098,21 +4161,21 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="46"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="106" t="s">
+      <c r="B3" s="115"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="103"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="103"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="108"/>
       <c r="J3" s="52" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="53">
-        <f>COUNTIF(M8:M1821,"Fail")</f>
+        <f>COUNTIF(M8:M1823,"Fail")</f>
         <v>0</v>
       </c>
       <c r="L3" s="51" t="s">
@@ -4127,25 +4190,25 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="46"/>
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="107" t="s">
+      <c r="C4" s="108"/>
+      <c r="D4" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="106" t="s">
+      <c r="E4" s="108"/>
+      <c r="F4" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="103"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="108"/>
       <c r="J4" s="49" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="54">
-        <f>COUNTIF(M9:M1821,"Out of Scope")</f>
+        <f>COUNTIF(M9:M1823,"Out of Scope")</f>
         <v>0</v>
       </c>
       <c r="L4" s="55" t="s">
@@ -4160,28 +4223,28 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="46"/>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="107" t="s">
+      <c r="C5" s="108"/>
+      <c r="D5" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="103"/>
-      <c r="F5" s="106" t="s">
+      <c r="E5" s="108"/>
+      <c r="F5" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="103"/>
-      <c r="H5" s="105" t="s">
+      <c r="G5" s="108"/>
+      <c r="H5" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="103"/>
+      <c r="I5" s="108"/>
       <c r="J5" s="56" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="57">
         <f>SUM(K2+K3+K4)</f>
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L5" s="51" t="s">
         <v>23</v>
@@ -4196,14 +4259,14 @@
     <row r="6" spans="1:26">
       <c r="A6" s="58"/>
       <c r="B6" s="58"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
       <c r="K6" s="58"/>
       <c r="L6" s="51" t="s">
         <v>24</v>
@@ -10127,7 +10190,7 @@
       <c r="A127" s="101" t="s">
         <v>667</v>
       </c>
-      <c r="B127" s="112" t="s">
+      <c r="B127" s="102" t="s">
         <v>668</v>
       </c>
       <c r="C127" s="61" t="s">
@@ -10167,32 +10230,44 @@
       <c r="Y127" s="36"/>
       <c r="Z127" s="36"/>
     </row>
-    <row r="128" spans="1:26" ht="66.599999999999994" thickBot="1">
-      <c r="A128" s="66" t="s">
+    <row r="128" spans="1:26" ht="79.8" thickBot="1">
+      <c r="A128" s="101" t="s">
         <v>667</v>
       </c>
-      <c r="B128" s="113" t="s">
+      <c r="B128" s="103" t="s">
         <v>671</v>
       </c>
-      <c r="C128" s="67"/>
-      <c r="D128" s="68" t="s">
+      <c r="C128" s="61" t="s">
+        <v>729</v>
+      </c>
+      <c r="D128" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="E128" s="69" t="s">
+      <c r="E128" s="63" t="s">
         <v>672</v>
       </c>
-      <c r="F128" s="67"/>
-      <c r="G128" s="70" t="s">
+      <c r="F128" s="61" t="s">
+        <v>730</v>
+      </c>
+      <c r="G128" s="64" t="s">
         <v>264</v>
       </c>
-      <c r="H128" s="67"/>
-      <c r="I128" s="67"/>
-      <c r="J128" s="67"/>
-      <c r="K128" s="67"/>
-      <c r="L128" s="71" t="s">
+      <c r="H128" s="61" t="s">
+        <v>731</v>
+      </c>
+      <c r="I128" s="61" t="s">
+        <v>732</v>
+      </c>
+      <c r="J128" s="79" t="s">
+        <v>733</v>
+      </c>
+      <c r="K128" s="61" t="s">
+        <v>734</v>
+      </c>
+      <c r="L128" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="M128" s="72" t="s">
+      <c r="M128" s="65" t="s">
         <v>41</v>
       </c>
       <c r="N128" s="36"/>
@@ -10209,15 +10284,15 @@
       <c r="Y128" s="36"/>
       <c r="Z128" s="36"/>
     </row>
-    <row r="129" spans="1:26" ht="409.6" thickBot="1">
-      <c r="A129" s="66" t="s">
-        <v>673</v>
-      </c>
-      <c r="B129" s="114" t="s">
-        <v>674</v>
+    <row r="129" spans="1:26" ht="79.8" thickBot="1">
+      <c r="A129" s="73">
+        <v>45659</v>
+      </c>
+      <c r="B129" s="103" t="s">
+        <v>735</v>
       </c>
       <c r="C129" s="67" t="s">
-        <v>675</v>
+        <v>736</v>
       </c>
       <c r="D129" s="68" t="s">
         <v>44</v>
@@ -10225,23 +10300,19 @@
       <c r="E129" s="69" t="s">
         <v>676</v>
       </c>
-      <c r="F129" s="115" t="s">
-        <v>677</v>
+      <c r="F129" s="67" t="s">
+        <v>737</v>
       </c>
       <c r="G129" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H129" s="67" t="s">
-        <v>678</v>
-      </c>
-      <c r="I129" s="67" t="s">
-        <v>679</v>
-      </c>
-      <c r="J129" s="76" t="s">
-        <v>680</v>
-      </c>
+        <v>738</v>
+      </c>
+      <c r="I129" s="67"/>
+      <c r="J129" s="67"/>
       <c r="K129" s="67" t="s">
-        <v>681</v>
+        <v>739</v>
       </c>
       <c r="L129" s="71" t="s">
         <v>50</v>
@@ -10263,13 +10334,15 @@
       <c r="Y129" s="36"/>
       <c r="Z129" s="36"/>
     </row>
-    <row r="130" spans="1:26" ht="66.599999999999994" thickBot="1">
-      <c r="A130" s="66"/>
-      <c r="B130" s="114" t="s">
-        <v>674</v>
+    <row r="130" spans="1:26" ht="79.8" thickBot="1">
+      <c r="A130" s="73">
+        <v>45660</v>
+      </c>
+      <c r="B130" s="103" t="s">
+        <v>735</v>
       </c>
       <c r="C130" s="67" t="s">
-        <v>675</v>
+        <v>740</v>
       </c>
       <c r="D130" s="68" t="s">
         <v>44</v>
@@ -10277,21 +10350,21 @@
       <c r="E130" s="69" t="s">
         <v>682</v>
       </c>
-      <c r="F130" s="115" t="s">
-        <v>683</v>
-      </c>
-      <c r="G130" s="70" t="s">
-        <v>264</v>
+      <c r="F130" s="67" t="s">
+        <v>741</v>
+      </c>
+      <c r="G130" s="75" t="s">
+        <v>64</v>
       </c>
       <c r="H130" s="67" t="s">
-        <v>684</v>
+        <v>742</v>
       </c>
       <c r="I130" s="67"/>
       <c r="J130" s="76" t="s">
-        <v>685</v>
+        <v>743</v>
       </c>
       <c r="K130" s="67" t="s">
-        <v>686</v>
+        <v>744</v>
       </c>
       <c r="L130" s="71" t="s">
         <v>50</v>
@@ -10313,37 +10386,39 @@
       <c r="Y130" s="36"/>
       <c r="Z130" s="36"/>
     </row>
-    <row r="131" spans="1:26" ht="264.60000000000002" thickBot="1">
-      <c r="A131" s="66"/>
-      <c r="B131" s="114" t="s">
+    <row r="131" spans="1:26" ht="409.6" thickBot="1">
+      <c r="A131" s="66" t="s">
+        <v>673</v>
+      </c>
+      <c r="B131" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C131" s="67" t="s">
-        <v>78</v>
+        <v>675</v>
       </c>
       <c r="D131" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E131" s="69" t="s">
-        <v>687</v>
-      </c>
-      <c r="F131" s="67" t="s">
-        <v>688</v>
+        <v>676</v>
+      </c>
+      <c r="F131" s="105" t="s">
+        <v>677</v>
       </c>
       <c r="G131" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H131" s="67" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="I131" s="67" t="s">
-        <v>690</v>
+        <v>679</v>
       </c>
       <c r="J131" s="76" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="K131" s="67" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
       <c r="L131" s="71" t="s">
         <v>50</v>
@@ -10365,37 +10440,35 @@
       <c r="Y131" s="36"/>
       <c r="Z131" s="36"/>
     </row>
-    <row r="132" spans="1:26" ht="93" thickBot="1">
+    <row r="132" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A132" s="66"/>
-      <c r="B132" s="114" t="s">
+      <c r="B132" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C132" s="67" t="s">
-        <v>78</v>
+        <v>675</v>
       </c>
       <c r="D132" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E132" s="69" t="s">
-        <v>693</v>
-      </c>
-      <c r="F132" s="67" t="s">
-        <v>694</v>
+        <v>682</v>
+      </c>
+      <c r="F132" s="105" t="s">
+        <v>683</v>
       </c>
       <c r="G132" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H132" s="67" t="s">
-        <v>695</v>
-      </c>
-      <c r="I132" s="67" t="s">
-        <v>696</v>
-      </c>
+        <v>684</v>
+      </c>
+      <c r="I132" s="67"/>
       <c r="J132" s="76" t="s">
-        <v>697</v>
+        <v>685</v>
       </c>
       <c r="K132" s="67" t="s">
-        <v>698</v>
+        <v>686</v>
       </c>
       <c r="L132" s="71" t="s">
         <v>50</v>
@@ -10417,37 +10490,37 @@
       <c r="Y132" s="36"/>
       <c r="Z132" s="36"/>
     </row>
-    <row r="133" spans="1:26" ht="211.8" thickBot="1">
+    <row r="133" spans="1:26" ht="264.60000000000002" thickBot="1">
       <c r="A133" s="66"/>
-      <c r="B133" s="114" t="s">
+      <c r="B133" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C133" s="67" t="s">
-        <v>699</v>
+        <v>78</v>
       </c>
       <c r="D133" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E133" s="69" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
       <c r="F133" s="67" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="G133" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H133" s="67" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
       <c r="I133" s="67" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="J133" s="76" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
       <c r="K133" s="67" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
       <c r="L133" s="71" t="s">
         <v>50</v>
@@ -10469,36 +10542,38 @@
       <c r="Y133" s="36"/>
       <c r="Z133" s="36"/>
     </row>
-    <row r="134" spans="1:26" ht="251.4" thickBot="1">
+    <row r="134" spans="1:26" ht="93" thickBot="1">
       <c r="A134" s="66"/>
-      <c r="B134" s="114" t="s">
+      <c r="B134" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C134" s="67" t="s">
-        <v>675</v>
+        <v>78</v>
       </c>
       <c r="D134" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E134" s="69" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
       <c r="F134" s="67" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
       <c r="G134" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H134" s="67" t="s">
-        <v>684</v>
+        <v>695</v>
       </c>
       <c r="I134" s="67" t="s">
-        <v>708</v>
+        <v>696</v>
       </c>
       <c r="J134" s="76" t="s">
-        <v>709</v>
-      </c>
-      <c r="K134" s="67"/>
+        <v>697</v>
+      </c>
+      <c r="K134" s="67" t="s">
+        <v>698</v>
+      </c>
       <c r="L134" s="71" t="s">
         <v>50</v>
       </c>
@@ -10519,37 +10594,37 @@
       <c r="Y134" s="36"/>
       <c r="Z134" s="36"/>
     </row>
-    <row r="135" spans="1:26" ht="225" thickBot="1">
+    <row r="135" spans="1:26" ht="211.8" thickBot="1">
       <c r="A135" s="66"/>
-      <c r="B135" s="114" t="s">
+      <c r="B135" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C135" s="67" t="s">
-        <v>710</v>
+        <v>699</v>
       </c>
       <c r="D135" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E135" s="69" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
       <c r="F135" s="67" t="s">
-        <v>712</v>
+        <v>701</v>
       </c>
       <c r="G135" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H135" s="67" t="s">
-        <v>713</v>
+        <v>702</v>
       </c>
       <c r="I135" s="67" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="J135" s="76" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
       <c r="K135" s="67" t="s">
-        <v>716</v>
+        <v>705</v>
       </c>
       <c r="L135" s="71" t="s">
         <v>50</v>
@@ -10571,38 +10646,36 @@
       <c r="Y135" s="36"/>
       <c r="Z135" s="36"/>
     </row>
-    <row r="136" spans="1:26" ht="145.80000000000001" thickBot="1">
+    <row r="136" spans="1:26" ht="251.4" thickBot="1">
       <c r="A136" s="66"/>
-      <c r="B136" s="114" t="s">
+      <c r="B136" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C136" s="67" t="s">
-        <v>717</v>
+        <v>675</v>
       </c>
       <c r="D136" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E136" s="69" t="s">
-        <v>718</v>
+        <v>706</v>
       </c>
       <c r="F136" s="67" t="s">
-        <v>719</v>
+        <v>707</v>
       </c>
       <c r="G136" s="70" t="s">
         <v>264</v>
       </c>
       <c r="H136" s="67" t="s">
-        <v>720</v>
+        <v>684</v>
       </c>
       <c r="I136" s="67" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
       <c r="J136" s="76" t="s">
-        <v>722</v>
-      </c>
-      <c r="K136" s="67" t="s">
-        <v>723</v>
-      </c>
+        <v>709</v>
+      </c>
+      <c r="K136" s="67"/>
       <c r="L136" s="71" t="s">
         <v>50</v>
       </c>
@@ -10623,35 +10696,37 @@
       <c r="Y136" s="36"/>
       <c r="Z136" s="36"/>
     </row>
-    <row r="137" spans="1:26" ht="119.4" thickBot="1">
+    <row r="137" spans="1:26" ht="225" thickBot="1">
       <c r="A137" s="66"/>
-      <c r="B137" s="116" t="s">
+      <c r="B137" s="104" t="s">
         <v>674</v>
       </c>
       <c r="C137" s="67" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="D137" s="68" t="s">
         <v>44</v>
       </c>
       <c r="E137" s="69" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="F137" s="67" t="s">
-        <v>726</v>
-      </c>
-      <c r="G137" s="75" t="s">
-        <v>64</v>
+        <v>712</v>
+      </c>
+      <c r="G137" s="70" t="s">
+        <v>264</v>
       </c>
       <c r="H137" s="67" t="s">
-        <v>684</v>
-      </c>
-      <c r="I137" s="67"/>
+        <v>713</v>
+      </c>
+      <c r="I137" s="67" t="s">
+        <v>714</v>
+      </c>
       <c r="J137" s="76" t="s">
-        <v>727</v>
+        <v>715</v>
       </c>
       <c r="K137" s="67" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
       <c r="L137" s="71" t="s">
         <v>50</v>
@@ -10673,45 +10748,107 @@
       <c r="Y137" s="36"/>
       <c r="Z137" s="36"/>
     </row>
-    <row r="138" spans="1:26">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
-      <c r="E138" s="4"/>
-      <c r="F138" s="4"/>
-      <c r="G138" s="4"/>
-      <c r="H138" s="4"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="4"/>
-      <c r="M138" s="4"/>
-      <c r="N138" s="4"/>
-      <c r="O138" s="4"/>
-      <c r="P138" s="4"/>
-      <c r="Q138" s="4"/>
-      <c r="R138" s="4"/>
-    </row>
-    <row r="139" spans="1:26">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
-      <c r="G139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
-      <c r="R139" s="4"/>
+    <row r="138" spans="1:26" ht="145.80000000000001" thickBot="1">
+      <c r="A138" s="66"/>
+      <c r="B138" s="104" t="s">
+        <v>674</v>
+      </c>
+      <c r="C138" s="67" t="s">
+        <v>717</v>
+      </c>
+      <c r="D138" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E138" s="69" t="s">
+        <v>718</v>
+      </c>
+      <c r="F138" s="67" t="s">
+        <v>719</v>
+      </c>
+      <c r="G138" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H138" s="67" t="s">
+        <v>720</v>
+      </c>
+      <c r="I138" s="67" t="s">
+        <v>721</v>
+      </c>
+      <c r="J138" s="76" t="s">
+        <v>722</v>
+      </c>
+      <c r="K138" s="67" t="s">
+        <v>723</v>
+      </c>
+      <c r="L138" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M138" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N138" s="36"/>
+      <c r="O138" s="36"/>
+      <c r="P138" s="36"/>
+      <c r="Q138" s="36"/>
+      <c r="R138" s="36"/>
+      <c r="S138" s="36"/>
+      <c r="T138" s="36"/>
+      <c r="U138" s="36"/>
+      <c r="V138" s="36"/>
+      <c r="W138" s="36"/>
+      <c r="X138" s="36"/>
+      <c r="Y138" s="36"/>
+      <c r="Z138" s="36"/>
+    </row>
+    <row r="139" spans="1:26" ht="119.4" thickBot="1">
+      <c r="A139" s="66"/>
+      <c r="B139" s="106" t="s">
+        <v>674</v>
+      </c>
+      <c r="C139" s="67" t="s">
+        <v>724</v>
+      </c>
+      <c r="D139" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E139" s="69" t="s">
+        <v>725</v>
+      </c>
+      <c r="F139" s="67" t="s">
+        <v>726</v>
+      </c>
+      <c r="G139" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="H139" s="67" t="s">
+        <v>684</v>
+      </c>
+      <c r="I139" s="67"/>
+      <c r="J139" s="76" t="s">
+        <v>727</v>
+      </c>
+      <c r="K139" s="67" t="s">
+        <v>728</v>
+      </c>
+      <c r="L139" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M139" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="N139" s="36"/>
+      <c r="O139" s="36"/>
+      <c r="P139" s="36"/>
+      <c r="Q139" s="36"/>
+      <c r="R139" s="36"/>
+      <c r="S139" s="36"/>
+      <c r="T139" s="36"/>
+      <c r="U139" s="36"/>
+      <c r="V139" s="36"/>
+      <c r="W139" s="36"/>
+      <c r="X139" s="36"/>
+      <c r="Y139" s="36"/>
+      <c r="Z139" s="36"/>
     </row>
     <row r="140" spans="1:26">
       <c r="A140" s="4"/>
@@ -27993,8 +28130,56 @@
       <c r="Q1003" s="4"/>
       <c r="R1003" s="4"/>
     </row>
+    <row r="1004" spans="1:18">
+      <c r="A1004" s="4"/>
+      <c r="B1004" s="4"/>
+      <c r="C1004" s="4"/>
+      <c r="D1004" s="4"/>
+      <c r="E1004" s="4"/>
+      <c r="F1004" s="4"/>
+      <c r="G1004" s="4"/>
+      <c r="H1004" s="4"/>
+      <c r="I1004" s="4"/>
+      <c r="J1004" s="4"/>
+      <c r="K1004" s="4"/>
+      <c r="L1004" s="4"/>
+      <c r="M1004" s="4"/>
+      <c r="N1004" s="4"/>
+      <c r="O1004" s="4"/>
+      <c r="P1004" s="4"/>
+      <c r="Q1004" s="4"/>
+      <c r="R1004" s="4"/>
+    </row>
+    <row r="1005" spans="1:18">
+      <c r="A1005" s="4"/>
+      <c r="B1005" s="4"/>
+      <c r="C1005" s="4"/>
+      <c r="D1005" s="4"/>
+      <c r="E1005" s="4"/>
+      <c r="F1005" s="4"/>
+      <c r="G1005" s="4"/>
+      <c r="H1005" s="4"/>
+      <c r="I1005" s="4"/>
+      <c r="J1005" s="4"/>
+      <c r="K1005" s="4"/>
+      <c r="L1005" s="4"/>
+      <c r="M1005" s="4"/>
+      <c r="N1005" s="4"/>
+      <c r="O1005" s="4"/>
+      <c r="P1005" s="4"/>
+      <c r="Q1005" s="4"/>
+      <c r="R1005" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -28009,14 +28194,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -28108,28 +28285,32 @@
     <hyperlink ref="B125" r:id="rId79" display="https://jira.ibos.io/browse/MGM-7651"/>
     <hyperlink ref="B126" r:id="rId80" display="https://jira.ibos.io/browse/MGM-7651"/>
     <hyperlink ref="B127" r:id="rId81" display="https://jira.ibos.io/browse/MGM-7162"/>
-    <hyperlink ref="B128" r:id="rId82" display="https://jira.ibos.io/browse/MGM-7873"/>
-    <hyperlink ref="B129" r:id="rId83" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J129" r:id="rId84"/>
-    <hyperlink ref="B130" r:id="rId85" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J130" r:id="rId86"/>
-    <hyperlink ref="B131" r:id="rId87" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J131" r:id="rId88"/>
-    <hyperlink ref="B132" r:id="rId89" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J132" r:id="rId90"/>
-    <hyperlink ref="B133" r:id="rId91" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J133" r:id="rId92"/>
-    <hyperlink ref="B134" r:id="rId93" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J134" r:id="rId94"/>
-    <hyperlink ref="B135" r:id="rId95" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J135" r:id="rId96"/>
-    <hyperlink ref="B136" r:id="rId97" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J136" r:id="rId98"/>
-    <hyperlink ref="B137" r:id="rId99" display="https://jira.ibos.io/browse/MGM-7861"/>
-    <hyperlink ref="J137" r:id="rId100"/>
+    <hyperlink ref="B131" r:id="rId82" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J131" r:id="rId83"/>
+    <hyperlink ref="B132" r:id="rId84" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J132" r:id="rId85"/>
+    <hyperlink ref="B133" r:id="rId86" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J133" r:id="rId87"/>
+    <hyperlink ref="B134" r:id="rId88" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J134" r:id="rId89"/>
+    <hyperlink ref="B135" r:id="rId90" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J135" r:id="rId91"/>
+    <hyperlink ref="B136" r:id="rId92" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J136" r:id="rId93"/>
+    <hyperlink ref="B137" r:id="rId94" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J137" r:id="rId95"/>
+    <hyperlink ref="B138" r:id="rId96" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J138" r:id="rId97"/>
+    <hyperlink ref="B139" r:id="rId98" display="https://jira.ibos.io/browse/MGM-7861"/>
+    <hyperlink ref="J139" r:id="rId99"/>
+    <hyperlink ref="B128" r:id="rId100" display="https://jira.ibos.io/browse/MGM-7873"/>
+    <hyperlink ref="J128" r:id="rId101"/>
+    <hyperlink ref="B129" r:id="rId102" display="https://jira.ibos.io/browse/MGM-7873"/>
+    <hyperlink ref="B130" r:id="rId103" display="https://jira.ibos.io/browse/MGM-7873"/>
+    <hyperlink ref="J130" r:id="rId104"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId101"/>
+  <pageSetup orientation="portrait" r:id="rId105"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Writing test case SKU based inventory report
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="813">
   <si>
     <t>Product Name</t>
   </si>
@@ -3121,6 +3121,132 @@
   </si>
   <si>
     <t>it will should be successfully sales Delivery then Sales order status complete</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7921</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Need to develop a new report (SKU Wise Stock Report) – Inventory Report</t>
+    </r>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Create item profile (UOM-PCS, Alt. UOM - Carton, Alt. Unit-20)</t>
+  </si>
+  <si>
+    <t>Configuration-item profile-UOM-PCS, Alt. UOM - Carton, Alt. Unit-20-save</t>
+  </si>
+  <si>
+    <t>UOM-PCS, Alt. UOM - Carton, Alt. Unit-20</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/B4Lo7ZTNM13b</t>
+  </si>
+  <si>
+    <t>it will should be successfully Created item profile</t>
+  </si>
+  <si>
+    <t>MGM-7921 configuration</t>
+  </si>
+  <si>
+    <t>standrad price</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>setup standrad price</t>
+  </si>
+  <si>
+    <t>Configuration- standrad price-save</t>
+  </si>
+  <si>
+    <t>Trading Price-9 
+Retails Price (MRP)-10</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/f-B2IyWSYmdD</t>
+  </si>
+  <si>
+    <t>it will should be setup standrad price</t>
+  </si>
+  <si>
+    <t>MGM-7921 Purchase</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>direct purchase receive item</t>
+  </si>
+  <si>
+    <t>purchase-purchase receive</t>
+  </si>
+  <si>
+    <t>it will should be direct purchase receive item</t>
+  </si>
+  <si>
+    <t>MGM-7921 sales</t>
+  </si>
+  <si>
+    <t>sales order</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>create sales order and approved</t>
+  </si>
+  <si>
+    <t>sales -sales order</t>
+  </si>
+  <si>
+    <t>it will should be created and approved sales order</t>
+  </si>
+  <si>
+    <t>sales delivery</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>sales -sales delivery</t>
+  </si>
+  <si>
+    <t>it will should be sales delivery</t>
+  </si>
+  <si>
+    <t>MGM-7921 inventory</t>
+  </si>
+  <si>
+    <t>inventory report</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inventory -inventory report-View By-SKU Wise Stock Report
+</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/_5a-IzIcJInk</t>
+  </si>
+  <si>
+    <t>it will should be inventory report-View By-SKU Wise Stock Report</t>
   </si>
 </sst>
 </file>
@@ -3940,32 +4066,32 @@
     <xf numFmtId="0" fontId="19" fillId="21" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4189,8 +4315,8 @@
   </sheetPr>
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T141" sqref="T141"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L143" sqref="L143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -4205,11 +4331,11 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="46"/>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="109" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="108"/>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="110" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="108"/>
@@ -4217,11 +4343,11 @@
         <v>2</v>
       </c>
       <c r="G1" s="108"/>
-      <c r="H1" s="116">
+      <c r="H1" s="113">
         <v>45615</v>
       </c>
       <c r="I1" s="108"/>
-      <c r="J1" s="114" t="s">
+      <c r="J1" s="107" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="108"/>
@@ -4237,11 +4363,11 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="46"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="109" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="108"/>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="110" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="108"/>
@@ -4249,14 +4375,14 @@
         <v>7</v>
       </c>
       <c r="G2" s="108"/>
-      <c r="H2" s="110"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="108"/>
       <c r="J2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="50">
         <f>COUNTIF(M8:M1823,"Pass")</f>
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L2" s="51" t="s">
         <v>9</v>
@@ -4270,15 +4396,15 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="46"/>
-      <c r="B3" s="109"/>
+      <c r="B3" s="115"/>
       <c r="C3" s="108"/>
-      <c r="D3" s="110"/>
+      <c r="D3" s="112"/>
       <c r="E3" s="108"/>
       <c r="F3" s="111" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="108"/>
-      <c r="H3" s="110"/>
+      <c r="H3" s="112"/>
       <c r="I3" s="108"/>
       <c r="J3" s="52" t="s">
         <v>11</v>
@@ -4299,11 +4425,11 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="46"/>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="108"/>
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="110" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="108"/>
@@ -4311,7 +4437,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="108"/>
-      <c r="H4" s="113"/>
+      <c r="H4" s="116"/>
       <c r="I4" s="108"/>
       <c r="J4" s="49" t="s">
         <v>16</v>
@@ -4332,11 +4458,11 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="46"/>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="109" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="108"/>
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="110" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="108"/>
@@ -4344,7 +4470,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="108"/>
-      <c r="H5" s="110" t="s">
+      <c r="H5" s="112" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="108"/>
@@ -4353,7 +4479,7 @@
       </c>
       <c r="K5" s="57">
         <f>SUM(K2+K3+K4)</f>
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L5" s="51" t="s">
         <v>23</v>
@@ -4368,7 +4494,7 @@
     <row r="6" spans="1:26">
       <c r="A6" s="58"/>
       <c r="B6" s="58"/>
-      <c r="C6" s="107"/>
+      <c r="C6" s="114"/>
       <c r="D6" s="108"/>
       <c r="E6" s="108"/>
       <c r="F6" s="108"/>
@@ -11185,120 +11311,262 @@
       <c r="Q144" s="4"/>
       <c r="R144" s="4"/>
     </row>
-    <row r="145" spans="1:18">
-      <c r="A145" s="4"/>
-      <c r="B145" s="4"/>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
-      <c r="E145" s="4"/>
-      <c r="F145" s="4"/>
-      <c r="G145" s="4"/>
-      <c r="H145" s="4"/>
-      <c r="I145" s="4"/>
-      <c r="J145" s="4"/>
-      <c r="K145" s="4"/>
-      <c r="L145" s="4"/>
-      <c r="M145" s="4"/>
+    <row r="145" spans="1:18" ht="106.2" thickBot="1">
+      <c r="A145" s="94">
+        <v>45664</v>
+      </c>
+      <c r="B145" s="74" t="s">
+        <v>776</v>
+      </c>
+      <c r="C145" s="61" t="s">
+        <v>777</v>
+      </c>
+      <c r="D145" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E145" s="63" t="s">
+        <v>778</v>
+      </c>
+      <c r="F145" s="61" t="s">
+        <v>779</v>
+      </c>
+      <c r="G145" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="H145" s="61" t="s">
+        <v>780</v>
+      </c>
+      <c r="I145" s="61" t="s">
+        <v>781</v>
+      </c>
+      <c r="J145" s="79" t="s">
+        <v>782</v>
+      </c>
+      <c r="K145" s="61" t="s">
+        <v>783</v>
+      </c>
+      <c r="L145" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="M145" s="65" t="s">
+        <v>41</v>
+      </c>
       <c r="N145" s="4"/>
       <c r="O145" s="4"/>
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
       <c r="R145" s="4"/>
     </row>
-    <row r="146" spans="1:18">
-      <c r="A146" s="4"/>
-      <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
-      <c r="E146" s="4"/>
-      <c r="F146" s="4"/>
-      <c r="G146" s="4"/>
-      <c r="H146" s="4"/>
-      <c r="I146" s="4"/>
-      <c r="J146" s="4"/>
-      <c r="K146" s="4"/>
-      <c r="L146" s="4"/>
-      <c r="M146" s="4"/>
+    <row r="146" spans="1:18" ht="53.4" thickBot="1">
+      <c r="A146" s="73">
+        <v>45664</v>
+      </c>
+      <c r="B146" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="C146" s="67" t="s">
+        <v>785</v>
+      </c>
+      <c r="D146" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E146" s="69" t="s">
+        <v>786</v>
+      </c>
+      <c r="F146" s="67" t="s">
+        <v>787</v>
+      </c>
+      <c r="G146" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H146" s="67" t="s">
+        <v>788</v>
+      </c>
+      <c r="I146" s="67" t="s">
+        <v>789</v>
+      </c>
+      <c r="J146" s="76" t="s">
+        <v>790</v>
+      </c>
+      <c r="K146" s="67" t="s">
+        <v>791</v>
+      </c>
+      <c r="L146" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M146" s="72" t="s">
+        <v>41</v>
+      </c>
       <c r="N146" s="4"/>
       <c r="O146" s="4"/>
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
       <c r="R146" s="4"/>
     </row>
-    <row r="147" spans="1:18">
-      <c r="A147" s="4"/>
-      <c r="B147" s="4"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
-      <c r="E147" s="4"/>
-      <c r="F147" s="4"/>
-      <c r="G147" s="4"/>
-      <c r="H147" s="4"/>
-      <c r="I147" s="4"/>
-      <c r="J147" s="4"/>
-      <c r="K147" s="4"/>
-      <c r="L147" s="4"/>
-      <c r="M147" s="4"/>
+    <row r="147" spans="1:18" ht="53.4" thickBot="1">
+      <c r="A147" s="73">
+        <v>45664</v>
+      </c>
+      <c r="B147" s="67" t="s">
+        <v>792</v>
+      </c>
+      <c r="C147" s="67" t="s">
+        <v>274</v>
+      </c>
+      <c r="D147" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E147" s="69" t="s">
+        <v>793</v>
+      </c>
+      <c r="F147" s="67" t="s">
+        <v>794</v>
+      </c>
+      <c r="G147" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H147" s="67" t="s">
+        <v>795</v>
+      </c>
+      <c r="I147" s="67"/>
+      <c r="J147" s="67"/>
+      <c r="K147" s="67" t="s">
+        <v>796</v>
+      </c>
+      <c r="L147" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M147" s="72" t="s">
+        <v>41</v>
+      </c>
       <c r="N147" s="4"/>
       <c r="O147" s="4"/>
       <c r="P147" s="4"/>
       <c r="Q147" s="4"/>
       <c r="R147" s="4"/>
     </row>
-    <row r="148" spans="1:18">
-      <c r="A148" s="4"/>
-      <c r="B148" s="4"/>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
-      <c r="E148" s="4"/>
-      <c r="F148" s="4"/>
-      <c r="G148" s="4"/>
-      <c r="H148" s="4"/>
-      <c r="I148" s="4"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="4"/>
-      <c r="M148" s="4"/>
+    <row r="148" spans="1:18" ht="53.4" thickBot="1">
+      <c r="A148" s="73">
+        <v>45664</v>
+      </c>
+      <c r="B148" s="67" t="s">
+        <v>797</v>
+      </c>
+      <c r="C148" s="67" t="s">
+        <v>798</v>
+      </c>
+      <c r="D148" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E148" s="69" t="s">
+        <v>799</v>
+      </c>
+      <c r="F148" s="67" t="s">
+        <v>800</v>
+      </c>
+      <c r="G148" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H148" s="67" t="s">
+        <v>801</v>
+      </c>
+      <c r="I148" s="67"/>
+      <c r="J148" s="67"/>
+      <c r="K148" s="67" t="s">
+        <v>802</v>
+      </c>
+      <c r="L148" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M148" s="72" t="s">
+        <v>41</v>
+      </c>
       <c r="N148" s="4"/>
       <c r="O148" s="4"/>
       <c r="P148" s="4"/>
       <c r="Q148" s="4"/>
       <c r="R148" s="4"/>
     </row>
-    <row r="149" spans="1:18">
-      <c r="A149" s="4"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
-      <c r="E149" s="4"/>
-      <c r="F149" s="4"/>
-      <c r="G149" s="4"/>
-      <c r="H149" s="4"/>
-      <c r="I149" s="4"/>
-      <c r="J149" s="4"/>
-      <c r="K149" s="4"/>
-      <c r="L149" s="4"/>
-      <c r="M149" s="4"/>
+    <row r="149" spans="1:18" ht="40.200000000000003" thickBot="1">
+      <c r="A149" s="73">
+        <v>45664</v>
+      </c>
+      <c r="B149" s="67" t="s">
+        <v>797</v>
+      </c>
+      <c r="C149" s="67" t="s">
+        <v>803</v>
+      </c>
+      <c r="D149" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E149" s="69" t="s">
+        <v>804</v>
+      </c>
+      <c r="F149" s="67" t="s">
+        <v>803</v>
+      </c>
+      <c r="G149" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H149" s="67" t="s">
+        <v>805</v>
+      </c>
+      <c r="I149" s="67"/>
+      <c r="J149" s="67"/>
+      <c r="K149" s="67" t="s">
+        <v>806</v>
+      </c>
+      <c r="L149" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M149" s="72" t="s">
+        <v>41</v>
+      </c>
       <c r="N149" s="4"/>
       <c r="O149" s="4"/>
       <c r="P149" s="4"/>
       <c r="Q149" s="4"/>
       <c r="R149" s="4"/>
     </row>
-    <row r="150" spans="1:18">
-      <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
-      <c r="E150" s="4"/>
-      <c r="F150" s="4"/>
-      <c r="G150" s="4"/>
-      <c r="H150" s="4"/>
-      <c r="I150" s="4"/>
-      <c r="J150" s="4"/>
-      <c r="K150" s="4"/>
-      <c r="L150" s="4"/>
-      <c r="M150" s="4"/>
+    <row r="150" spans="1:18" ht="66.599999999999994" thickBot="1">
+      <c r="A150" s="73">
+        <v>45664</v>
+      </c>
+      <c r="B150" s="67" t="s">
+        <v>807</v>
+      </c>
+      <c r="C150" s="67" t="s">
+        <v>808</v>
+      </c>
+      <c r="D150" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E150" s="69" t="s">
+        <v>809</v>
+      </c>
+      <c r="F150" s="67" t="s">
+        <v>808</v>
+      </c>
+      <c r="G150" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="H150" s="67" t="s">
+        <v>810</v>
+      </c>
+      <c r="I150" s="67"/>
+      <c r="J150" s="76" t="s">
+        <v>811</v>
+      </c>
+      <c r="K150" s="67" t="s">
+        <v>812</v>
+      </c>
+      <c r="L150" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M150" s="72" t="s">
+        <v>41</v>
+      </c>
       <c r="N150" s="4"/>
       <c r="O150" s="4"/>
       <c r="P150" s="4"/>
@@ -28407,6 +28675,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -28421,14 +28697,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -28552,9 +28820,13 @@
     <hyperlink ref="J143" r:id="rId111"/>
     <hyperlink ref="B144" r:id="rId112" display="https://jira.ibos.io/browse/MGM-7825"/>
     <hyperlink ref="J144" r:id="rId113"/>
+    <hyperlink ref="B145" r:id="rId114" display="https://jira.ibos.io/browse/MGM-7921"/>
+    <hyperlink ref="J145" r:id="rId115"/>
+    <hyperlink ref="J146" r:id="rId116"/>
+    <hyperlink ref="J150" r:id="rId117"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId114"/>
+  <pageSetup orientation="portrait" r:id="rId118"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
test case in purchase payment
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10632" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10632"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="926">
   <si>
     <t>Product Name</t>
   </si>
@@ -3466,6 +3466,178 @@
   </si>
   <si>
     <t>After delete this paid Bill we couldn't create new bill against the same GRN.</t>
+  </si>
+  <si>
+    <t>-M250100246</t>
+  </si>
+  <si>
+    <t>TC_139</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/QSlpwDZiWRcT</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-8400</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Customer Sales (Details)</t>
+    </r>
+  </si>
+  <si>
+    <t>Sales Analytics</t>
+  </si>
+  <si>
+    <t>TC_140</t>
+  </si>
+  <si>
+    <t>Try to checking sales analytics &amp; report Column Renamed Required -Customer Sales (Details)</t>
+  </si>
+  <si>
+    <t>Sales-&gt; Sales Analytics-&gt;Customer Sales (Details)-&gt;click Amaount only-&gt; view</t>
+  </si>
+  <si>
+    <t>It will should be Column Renamed Required -Customer Sales (Details)</t>
+  </si>
+  <si>
+    <t>TC_141</t>
+  </si>
+  <si>
+    <t>Try to checking sales analytics &amp; report Column name Required -Customer Sales (Details) and the Excel file Column name.</t>
+  </si>
+  <si>
+    <t>Sales-&gt; Sales Analytics-&gt;Customer Sales (Details)-&gt;click Amaount only-&gt; view-&gt;excel</t>
+  </si>
+  <si>
+    <t>It will should be sales analytics &amp; report Column name Required wise Customer Sales (Details) and the Excel file Column name.</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-7609</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Production Details Report</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_142</t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-8602</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Purchase Payment </t>
+    </r>
+  </si>
+  <si>
+    <t>Purchase Order</t>
+  </si>
+  <si>
+    <t>TC_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create Purchase Order
+</t>
+  </si>
+  <si>
+    <t>Purchase -&gt;Purchase Order-&gt;Create Purchase Order-add iem-&gt;save</t>
+  </si>
+  <si>
+    <t>Item Name: yttt-red/M 
+Order Qty: 3 
+Rate : 10</t>
+  </si>
+  <si>
+    <t>it will should be successfully Created Purchase Order</t>
+  </si>
+  <si>
+    <t>TC_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Purchase Receive
+</t>
+  </si>
+  <si>
+    <t>Purchase-&gt;Purchase Receive-&gt;Actions-Receive</t>
+  </si>
+  <si>
+    <t>Office: MGM Head Office</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/jSsP3UvjAJYV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it will should be successfully Purchase Receive
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Payment
+</t>
+  </si>
+  <si>
+    <t>TC_145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create Supplier Bill
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Payment-&gt; Create Supplier Bill-&gt;Select PO-&gt;save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office: MGM Head Office
+PO No.: PO-M250200101 
+</t>
+  </si>
+  <si>
+    <t>it will should be successfully Create Supplier Bill-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Payment 
+</t>
+  </si>
+  <si>
+    <t>TC_146</t>
+  </si>
+  <si>
+    <t>Try to shwoing PO and GRN in pending bill page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Payment-&gt; pending bill
+</t>
+  </si>
+  <si>
+    <t>https://prnt.sc/hRESRJNdLYrX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it will should be successfully shwoing PO and GRN in pending bill
+</t>
   </si>
 </sst>
 </file>
@@ -4264,34 +4436,6 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4417,6 +4561,34 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4639,8 +4811,8 @@
   </sheetPr>
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L143" sqref="L143"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S157" sqref="S157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -4655,26 +4827,26 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="15"/>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="81" t="s">
+      <c r="C1" s="119"/>
+      <c r="D1" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="80" t="s">
+      <c r="E1" s="119"/>
+      <c r="F1" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="85">
+      <c r="G1" s="119"/>
+      <c r="H1" s="124">
         <v>45615</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="83" t="s">
+      <c r="I1" s="119"/>
+      <c r="J1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="77"/>
+      <c r="K1" s="119"/>
       <c r="L1" s="16"/>
       <c r="M1" s="17" t="s">
         <v>4</v>
@@ -4687,26 +4859,26 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="15"/>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="81" t="s">
+      <c r="C2" s="119"/>
+      <c r="D2" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="80" t="s">
+      <c r="E2" s="119"/>
+      <c r="F2" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="77"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="119"/>
       <c r="J2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="19">
         <f>COUNTIF(M8:M1823,"Pass")</f>
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>9</v>
@@ -4720,16 +4892,16 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="15"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="80" t="s">
+      <c r="B3" s="126"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="77"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="119"/>
       <c r="J3" s="21" t="s">
         <v>11</v>
       </c>
@@ -4749,20 +4921,20 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="15"/>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="81" t="s">
+      <c r="C4" s="119"/>
+      <c r="D4" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="80" t="s">
+      <c r="E4" s="119"/>
+      <c r="F4" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="77"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="119"/>
       <c r="J4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4782,28 +4954,28 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="15"/>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="81" t="s">
+      <c r="C5" s="119"/>
+      <c r="D5" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="80" t="s">
+      <c r="E5" s="119"/>
+      <c r="F5" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="H5" s="79" t="s">
+      <c r="G5" s="119"/>
+      <c r="H5" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="77"/>
+      <c r="I5" s="119"/>
       <c r="J5" s="25" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="26">
         <f>SUM(K2+K3+K4)</f>
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L5" s="20" t="s">
         <v>23</v>
@@ -4818,14 +4990,14 @@
     <row r="6" spans="1:26">
       <c r="A6" s="27"/>
       <c r="B6" s="27"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
       <c r="K6" s="27"/>
       <c r="L6" s="20" t="s">
         <v>24</v>
@@ -11897,160 +12069,332 @@
       <c r="Q150" s="4"/>
       <c r="R150" s="4"/>
     </row>
-    <row r="151" spans="1:18">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
-      <c r="E151" s="4"/>
-      <c r="F151" s="4"/>
-      <c r="G151" s="4"/>
-      <c r="H151" s="4"/>
-      <c r="I151" s="4"/>
-      <c r="J151" s="4"/>
-      <c r="K151" s="4"/>
-      <c r="L151" s="4"/>
-      <c r="M151" s="4"/>
+    <row r="151" spans="1:18" ht="40.200000000000003" thickBot="1">
+      <c r="A151" s="63">
+        <v>45677</v>
+      </c>
+      <c r="B151" s="30" t="s">
+        <v>886</v>
+      </c>
+      <c r="C151" s="30" t="s">
+        <v>541</v>
+      </c>
+      <c r="D151" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E151" s="32" t="s">
+        <v>887</v>
+      </c>
+      <c r="F151" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="G151" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="H151" s="30"/>
+      <c r="I151" s="30"/>
+      <c r="J151" s="48" t="s">
+        <v>888</v>
+      </c>
+      <c r="K151" s="30"/>
+      <c r="L151" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="M151" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="N151" s="4"/>
       <c r="O151" s="4"/>
       <c r="P151" s="4"/>
       <c r="Q151" s="4"/>
       <c r="R151" s="4"/>
     </row>
-    <row r="152" spans="1:18">
-      <c r="A152" s="4"/>
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
-      <c r="E152" s="4"/>
-      <c r="F152" s="4"/>
-      <c r="G152" s="4"/>
-      <c r="H152" s="4"/>
-      <c r="I152" s="4"/>
-      <c r="J152" s="4"/>
-      <c r="K152" s="4"/>
-      <c r="L152" s="4"/>
-      <c r="M152" s="4"/>
+    <row r="152" spans="1:18" ht="93" thickBot="1">
+      <c r="A152" s="42">
+        <v>45694</v>
+      </c>
+      <c r="B152" s="43" t="s">
+        <v>889</v>
+      </c>
+      <c r="C152" s="36" t="s">
+        <v>890</v>
+      </c>
+      <c r="D152" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E152" s="38" t="s">
+        <v>891</v>
+      </c>
+      <c r="F152" s="36" t="s">
+        <v>892</v>
+      </c>
+      <c r="G152" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H152" s="36" t="s">
+        <v>893</v>
+      </c>
+      <c r="I152" s="36"/>
+      <c r="J152" s="36"/>
+      <c r="K152" s="36" t="s">
+        <v>894</v>
+      </c>
+      <c r="L152" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M152" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N152" s="4"/>
       <c r="O152" s="4"/>
       <c r="P152" s="4"/>
       <c r="Q152" s="4"/>
       <c r="R152" s="4"/>
     </row>
-    <row r="153" spans="1:18">
-      <c r="A153" s="4"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
-      <c r="D153" s="4"/>
-      <c r="E153" s="4"/>
-      <c r="F153" s="4"/>
-      <c r="G153" s="4"/>
-      <c r="H153" s="4"/>
-      <c r="I153" s="4"/>
-      <c r="J153" s="4"/>
-      <c r="K153" s="4"/>
-      <c r="L153" s="4"/>
-      <c r="M153" s="4"/>
+    <row r="153" spans="1:18" ht="159" thickBot="1">
+      <c r="A153" s="42">
+        <v>45694</v>
+      </c>
+      <c r="B153" s="43" t="s">
+        <v>889</v>
+      </c>
+      <c r="C153" s="36" t="s">
+        <v>890</v>
+      </c>
+      <c r="D153" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E153" s="38" t="s">
+        <v>895</v>
+      </c>
+      <c r="F153" s="36" t="s">
+        <v>896</v>
+      </c>
+      <c r="G153" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H153" s="36" t="s">
+        <v>897</v>
+      </c>
+      <c r="I153" s="36"/>
+      <c r="J153" s="36"/>
+      <c r="K153" s="36" t="s">
+        <v>898</v>
+      </c>
+      <c r="L153" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M153" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N153" s="4"/>
       <c r="O153" s="4"/>
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
       <c r="R153" s="4"/>
     </row>
-    <row r="154" spans="1:18">
-      <c r="A154" s="4"/>
-      <c r="B154" s="4"/>
-      <c r="C154" s="4"/>
-      <c r="D154" s="4"/>
-      <c r="E154" s="4"/>
-      <c r="F154" s="4"/>
-      <c r="G154" s="4"/>
-      <c r="H154" s="4"/>
-      <c r="I154" s="4"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
-      <c r="L154" s="4"/>
-      <c r="M154" s="4"/>
+    <row r="154" spans="1:18" ht="40.200000000000003" thickBot="1">
+      <c r="A154" s="42">
+        <v>45694</v>
+      </c>
+      <c r="B154" s="43" t="s">
+        <v>899</v>
+      </c>
+      <c r="C154" s="36" t="s">
+        <v>582</v>
+      </c>
+      <c r="D154" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E154" s="38" t="s">
+        <v>900</v>
+      </c>
+      <c r="F154" s="36"/>
+      <c r="G154" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H154" s="36"/>
+      <c r="I154" s="36"/>
+      <c r="J154" s="36"/>
+      <c r="K154" s="36"/>
+      <c r="L154" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M154" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N154" s="4"/>
       <c r="O154" s="4"/>
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
       <c r="R154" s="4"/>
     </row>
-    <row r="155" spans="1:18">
-      <c r="A155" s="4"/>
-      <c r="B155" s="4"/>
-      <c r="C155" s="4"/>
-      <c r="D155" s="4"/>
-      <c r="E155" s="4"/>
-      <c r="F155" s="4"/>
-      <c r="G155" s="4"/>
-      <c r="H155" s="4"/>
-      <c r="I155" s="4"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
-      <c r="L155" s="4"/>
-      <c r="M155" s="4"/>
+    <row r="155" spans="1:18" ht="79.8" thickBot="1">
+      <c r="A155" s="42">
+        <v>45701</v>
+      </c>
+      <c r="B155" s="43" t="s">
+        <v>901</v>
+      </c>
+      <c r="C155" s="36" t="s">
+        <v>902</v>
+      </c>
+      <c r="D155" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E155" s="38" t="s">
+        <v>903</v>
+      </c>
+      <c r="F155" s="36" t="s">
+        <v>904</v>
+      </c>
+      <c r="G155" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H155" s="36" t="s">
+        <v>905</v>
+      </c>
+      <c r="I155" s="36" t="s">
+        <v>906</v>
+      </c>
+      <c r="J155" s="36"/>
+      <c r="K155" s="36" t="s">
+        <v>907</v>
+      </c>
+      <c r="L155" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M155" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N155" s="4"/>
       <c r="O155" s="4"/>
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
       <c r="R155" s="4"/>
     </row>
-    <row r="156" spans="1:18">
-      <c r="A156" s="4"/>
-      <c r="B156" s="4"/>
-      <c r="C156" s="4"/>
-      <c r="D156" s="4"/>
-      <c r="E156" s="4"/>
-      <c r="F156" s="4"/>
-      <c r="G156" s="4"/>
-      <c r="H156" s="4"/>
-      <c r="I156" s="4"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
-      <c r="L156" s="4"/>
-      <c r="M156" s="4"/>
+    <row r="156" spans="1:18" ht="79.8" thickBot="1">
+      <c r="A156" s="35"/>
+      <c r="B156" s="43" t="s">
+        <v>901</v>
+      </c>
+      <c r="C156" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="D156" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E156" s="38" t="s">
+        <v>908</v>
+      </c>
+      <c r="F156" s="36" t="s">
+        <v>909</v>
+      </c>
+      <c r="G156" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H156" s="36" t="s">
+        <v>910</v>
+      </c>
+      <c r="I156" s="36" t="s">
+        <v>911</v>
+      </c>
+      <c r="J156" s="45" t="s">
+        <v>912</v>
+      </c>
+      <c r="K156" s="36" t="s">
+        <v>913</v>
+      </c>
+      <c r="L156" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M156" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N156" s="4"/>
       <c r="O156" s="4"/>
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
       <c r="R156" s="4"/>
     </row>
-    <row r="157" spans="1:18">
-      <c r="A157" s="4"/>
-      <c r="B157" s="4"/>
-      <c r="C157" s="4"/>
-      <c r="D157" s="4"/>
-      <c r="E157" s="4"/>
-      <c r="F157" s="4"/>
-      <c r="G157" s="4"/>
-      <c r="H157" s="4"/>
-      <c r="I157" s="4"/>
-      <c r="J157" s="4"/>
-      <c r="K157" s="4"/>
-      <c r="L157" s="4"/>
-      <c r="M157" s="4"/>
+    <row r="157" spans="1:18" ht="66.599999999999994" thickBot="1">
+      <c r="A157" s="35"/>
+      <c r="B157" s="43" t="s">
+        <v>901</v>
+      </c>
+      <c r="C157" s="36" t="s">
+        <v>914</v>
+      </c>
+      <c r="D157" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E157" s="38" t="s">
+        <v>915</v>
+      </c>
+      <c r="F157" s="36" t="s">
+        <v>916</v>
+      </c>
+      <c r="G157" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H157" s="36" t="s">
+        <v>917</v>
+      </c>
+      <c r="I157" s="36" t="s">
+        <v>918</v>
+      </c>
+      <c r="J157" s="36"/>
+      <c r="K157" s="36" t="s">
+        <v>919</v>
+      </c>
+      <c r="L157" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M157" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N157" s="4"/>
       <c r="O157" s="4"/>
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
       <c r="R157" s="4"/>
     </row>
-    <row r="158" spans="1:18">
-      <c r="A158" s="4"/>
-      <c r="B158" s="4"/>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4"/>
-      <c r="E158" s="4"/>
-      <c r="F158" s="4"/>
-      <c r="G158" s="4"/>
-      <c r="H158" s="4"/>
-      <c r="I158" s="4"/>
-      <c r="J158" s="4"/>
-      <c r="K158" s="4"/>
-      <c r="L158" s="4"/>
-      <c r="M158" s="4"/>
+    <row r="158" spans="1:18" ht="93" thickBot="1">
+      <c r="A158" s="35"/>
+      <c r="B158" s="43" t="s">
+        <v>901</v>
+      </c>
+      <c r="C158" s="36" t="s">
+        <v>920</v>
+      </c>
+      <c r="D158" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E158" s="38" t="s">
+        <v>921</v>
+      </c>
+      <c r="F158" s="36" t="s">
+        <v>922</v>
+      </c>
+      <c r="G158" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H158" s="36" t="s">
+        <v>923</v>
+      </c>
+      <c r="I158" s="36"/>
+      <c r="J158" s="45" t="s">
+        <v>924</v>
+      </c>
+      <c r="K158" s="36" t="s">
+        <v>925</v>
+      </c>
+      <c r="L158" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M158" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N158" s="4"/>
       <c r="O158" s="4"/>
       <c r="P158" s="4"/>
@@ -28999,6 +29343,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -29013,14 +29365,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -29148,9 +29492,19 @@
     <hyperlink ref="J145" r:id="rId115"/>
     <hyperlink ref="J146" r:id="rId116"/>
     <hyperlink ref="J150" r:id="rId117"/>
+    <hyperlink ref="J151" r:id="rId118"/>
+    <hyperlink ref="B152" r:id="rId119" display="https://jira.ibos.io/browse/MGM-8400"/>
+    <hyperlink ref="B153" r:id="rId120" display="https://jira.ibos.io/browse/MGM-8400"/>
+    <hyperlink ref="B154" r:id="rId121" display="https://jira.ibos.io/browse/MGM-7609"/>
+    <hyperlink ref="B155" r:id="rId122" display="https://jira.ibos.io/browse/MGM-8602"/>
+    <hyperlink ref="B156" r:id="rId123" display="https://jira.ibos.io/browse/MGM-8602"/>
+    <hyperlink ref="J156" r:id="rId124"/>
+    <hyperlink ref="B157" r:id="rId125" display="https://jira.ibos.io/browse/MGM-8602"/>
+    <hyperlink ref="B158" r:id="rId126" display="https://jira.ibos.io/browse/MGM-8602"/>
+    <hyperlink ref="J158" r:id="rId127"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId118"/>
+  <pageSetup orientation="portrait" r:id="rId128"/>
 </worksheet>
 </file>
 
@@ -29161,7 +29515,7 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -29172,40 +29526,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="76" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="87">
+      <c r="B1" s="77">
         <v>2</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="79" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="77" t="s">
         <v>243</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="80" t="s">
         <v>810</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="K1" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="L1" s="92"/>
+      <c r="L1" s="82"/>
       <c r="M1" s="60"/>
       <c r="N1" s="60"/>
       <c r="O1" s="60"/>
@@ -29222,17 +29576,17 @@
       <c r="Z1" s="60"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="94">
+      <c r="B2" s="84">
         <v>45411</v>
       </c>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="85" t="s">
         <v>247</v>
       </c>
       <c r="D2" s="40"/>
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="86" t="s">
         <v>811</v>
       </c>
       <c r="F2" s="40"/>
@@ -29240,10 +29594,10 @@
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
       <c r="J2" s="40"/>
-      <c r="K2" s="97" t="s">
+      <c r="K2" s="87" t="s">
         <v>248</v>
       </c>
-      <c r="L2" s="98">
+      <c r="L2" s="88">
         <v>45412</v>
       </c>
       <c r="M2" s="60"/>
@@ -29262,7 +29616,7 @@
       <c r="Z2" s="60"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="83" t="s">
         <v>812</v>
       </c>
       <c r="B3" s="40"/>
@@ -29274,10 +29628,10 @@
       <c r="H3" s="40"/>
       <c r="I3" s="40"/>
       <c r="J3" s="40"/>
-      <c r="K3" s="99" t="s">
+      <c r="K3" s="89" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="100">
+      <c r="L3" s="90">
         <v>1</v>
       </c>
       <c r="M3" s="60"/>
@@ -29296,36 +29650,36 @@
       <c r="Z3" s="60"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="83" t="s">
         <v>813</v>
       </c>
-      <c r="B4" s="94">
+      <c r="B4" s="84">
         <v>45622</v>
       </c>
       <c r="C4" s="68"/>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="91" t="s">
         <v>250</v>
       </c>
       <c r="E4" s="40"/>
-      <c r="F4" s="102" t="s">
+      <c r="F4" s="92" t="s">
         <v>251</v>
       </c>
-      <c r="G4" s="103" t="s">
+      <c r="G4" s="93" t="s">
         <v>252</v>
       </c>
-      <c r="H4" s="104" t="s">
+      <c r="H4" s="94" t="s">
         <v>253</v>
       </c>
-      <c r="I4" s="105" t="s">
+      <c r="I4" s="95" t="s">
         <v>254</v>
       </c>
-      <c r="J4" s="106" t="s">
+      <c r="J4" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="K4" s="99" t="s">
+      <c r="K4" s="89" t="s">
         <v>256</v>
       </c>
-      <c r="L4" s="100">
+      <c r="L4" s="90">
         <v>17</v>
       </c>
       <c r="M4" s="60"/>
@@ -29344,40 +29698,40 @@
       <c r="Z4" s="60"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="83" t="s">
         <v>814</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="97" t="s">
         <v>815</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="98" t="s">
         <v>816</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E5" s="101" t="s">
+      <c r="E5" s="91" t="s">
         <v>817</v>
       </c>
-      <c r="F5" s="102" t="s">
+      <c r="F5" s="92" t="s">
         <v>251</v>
       </c>
-      <c r="G5" s="103" t="s">
+      <c r="G5" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H5" s="109" t="s">
+      <c r="H5" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I5" s="110" t="s">
+      <c r="I5" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="J5" s="101" t="s">
+      <c r="J5" s="91" t="s">
         <v>819</v>
       </c>
-      <c r="K5" s="111" t="s">
+      <c r="K5" s="101" t="s">
         <v>820</v>
       </c>
-      <c r="L5" s="112"/>
+      <c r="L5" s="102"/>
       <c r="M5" s="60"/>
       <c r="N5" s="60"/>
       <c r="O5" s="60"/>
@@ -29394,40 +29748,40 @@
       <c r="Z5" s="60"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="83" t="s">
         <v>821</v>
       </c>
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="97" t="s">
         <v>815</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="98" t="s">
         <v>822</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E6" s="101" t="s">
+      <c r="E6" s="91" t="s">
         <v>823</v>
       </c>
-      <c r="F6" s="102" t="s">
+      <c r="F6" s="92" t="s">
         <v>251</v>
       </c>
-      <c r="G6" s="103" t="s">
+      <c r="G6" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I6" s="110" t="s">
+      <c r="I6" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="J6" s="101" t="s">
+      <c r="J6" s="91" t="s">
         <v>819</v>
       </c>
-      <c r="K6" s="113" t="s">
+      <c r="K6" s="103" t="s">
         <v>257</v>
       </c>
-      <c r="L6" s="114">
+      <c r="L6" s="104">
         <v>13</v>
       </c>
       <c r="M6" s="60"/>
@@ -29446,40 +29800,40 @@
       <c r="Z6" s="60"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="83" t="s">
         <v>824</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="97" t="s">
         <v>815</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="98" t="s">
         <v>825</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="91" t="s">
         <v>826</v>
       </c>
-      <c r="F7" s="102" t="s">
+      <c r="F7" s="92" t="s">
         <v>251</v>
       </c>
-      <c r="G7" s="103" t="s">
+      <c r="G7" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I7" s="110" t="s">
+      <c r="I7" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="J7" s="101" t="s">
+      <c r="J7" s="91" t="s">
         <v>819</v>
       </c>
-      <c r="K7" s="115" t="s">
+      <c r="K7" s="105" t="s">
         <v>251</v>
       </c>
-      <c r="L7" s="116">
+      <c r="L7" s="106">
         <v>4</v>
       </c>
       <c r="M7" s="60"/>
@@ -29498,40 +29852,40 @@
       <c r="Z7" s="60"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="83" t="s">
         <v>827</v>
       </c>
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="97" t="s">
         <v>815</v>
       </c>
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="98" t="s">
         <v>828</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E8" s="101" t="s">
+      <c r="E8" s="91" t="s">
         <v>829</v>
       </c>
-      <c r="F8" s="117" t="s">
+      <c r="F8" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G8" s="103" t="s">
+      <c r="G8" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H8" s="109" t="s">
+      <c r="H8" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I8" s="118" t="s">
+      <c r="I8" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="91" t="s">
         <v>831</v>
       </c>
-      <c r="K8" s="119" t="s">
+      <c r="K8" s="109" t="s">
         <v>258</v>
       </c>
-      <c r="L8" s="120">
+      <c r="L8" s="110">
         <v>1</v>
       </c>
       <c r="M8" s="60"/>
@@ -29550,40 +29904,40 @@
       <c r="Z8" s="60"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="83" t="s">
         <v>832</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="97" t="s">
         <v>833</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="98" t="s">
         <v>834</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E9" s="101" t="s">
+      <c r="E9" s="91" t="s">
         <v>835</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G9" s="103" t="s">
+      <c r="G9" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="H9" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I9" s="118" t="s">
+      <c r="I9" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J9" s="101" t="s">
+      <c r="J9" s="91" t="s">
         <v>836</v>
       </c>
-      <c r="K9" s="121" t="s">
+      <c r="K9" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="L9" s="100">
+      <c r="L9" s="90">
         <v>0</v>
       </c>
       <c r="M9" s="60"/>
@@ -29602,38 +29956,38 @@
       <c r="Z9" s="60"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="83" t="s">
         <v>837</v>
       </c>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="97" t="s">
         <v>838</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="98" t="s">
         <v>839</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="91" t="s">
         <v>840</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G10" s="103" t="s">
+      <c r="G10" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H10" s="109" t="s">
+      <c r="H10" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I10" s="118" t="s">
+      <c r="I10" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J10" s="101" t="s">
+      <c r="J10" s="91" t="s">
         <v>831</v>
       </c>
       <c r="K10" s="68"/>
-      <c r="L10" s="122"/>
+      <c r="L10" s="112"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
@@ -29650,34 +30004,34 @@
       <c r="Z10" s="60"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="83" t="s">
         <v>841</v>
       </c>
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="97" t="s">
         <v>842</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="98" t="s">
         <v>843</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="113" t="s">
         <v>844</v>
       </c>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G11" s="103" t="s">
+      <c r="G11" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H11" s="109" t="s">
+      <c r="H11" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I11" s="118" t="s">
+      <c r="I11" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J11" s="101" t="s">
+      <c r="J11" s="91" t="s">
         <v>831</v>
       </c>
       <c r="K11" s="40"/>
@@ -29698,34 +30052,34 @@
       <c r="Z11" s="60"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="83" t="s">
         <v>845</v>
       </c>
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="97" t="s">
         <v>846</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="98" t="s">
         <v>847</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E12" s="123" t="s">
+      <c r="E12" s="113" t="s">
         <v>848</v>
       </c>
-      <c r="F12" s="117" t="s">
+      <c r="F12" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G12" s="103" t="s">
+      <c r="G12" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H12" s="109" t="s">
+      <c r="H12" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I12" s="118" t="s">
+      <c r="I12" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J12" s="101" t="s">
+      <c r="J12" s="91" t="s">
         <v>831</v>
       </c>
       <c r="K12" s="40"/>
@@ -29746,34 +30100,34 @@
       <c r="Z12" s="60"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="83" t="s">
         <v>849</v>
       </c>
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="97" t="s">
         <v>850</v>
       </c>
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="98" t="s">
         <v>851</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="91" t="s">
         <v>852</v>
       </c>
-      <c r="F13" s="117" t="s">
+      <c r="F13" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G13" s="103" t="s">
+      <c r="G13" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H13" s="109" t="s">
+      <c r="H13" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I13" s="118" t="s">
+      <c r="I13" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J13" s="101" t="s">
+      <c r="J13" s="91" t="s">
         <v>853</v>
       </c>
       <c r="K13" s="60"/>
@@ -29794,34 +30148,34 @@
       <c r="Z13" s="60"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="83" t="s">
         <v>854</v>
       </c>
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="97" t="s">
         <v>855</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="98" t="s">
         <v>856</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E14" s="101" t="s">
+      <c r="E14" s="91" t="s">
         <v>857</v>
       </c>
-      <c r="F14" s="117" t="s">
+      <c r="F14" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G14" s="103" t="s">
+      <c r="G14" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H14" s="109" t="s">
+      <c r="H14" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I14" s="118" t="s">
+      <c r="I14" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J14" s="124" t="s">
+      <c r="J14" s="114" t="s">
         <v>255</v>
       </c>
       <c r="K14" s="60"/>
@@ -29842,34 +30196,34 @@
       <c r="Z14" s="60"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="93" t="s">
+      <c r="A15" s="83" t="s">
         <v>858</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="97" t="s">
         <v>859</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="98" t="s">
         <v>860</v>
       </c>
-      <c r="D15" s="101" t="s">
+      <c r="D15" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="91" t="s">
         <v>861</v>
       </c>
-      <c r="F15" s="117" t="s">
+      <c r="F15" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G15" s="103" t="s">
+      <c r="G15" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H15" s="109" t="s">
+      <c r="H15" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I15" s="118" t="s">
+      <c r="I15" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="91" t="s">
         <v>862</v>
       </c>
       <c r="K15" s="60"/>
@@ -29890,34 +30244,34 @@
       <c r="Z15" s="60"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="83" t="s">
         <v>863</v>
       </c>
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="97" t="s">
         <v>864</v>
       </c>
-      <c r="C16" s="108" t="s">
+      <c r="C16" s="98" t="s">
         <v>865</v>
       </c>
-      <c r="D16" s="101" t="s">
+      <c r="D16" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="101" t="s">
+      <c r="E16" s="91" t="s">
         <v>866</v>
       </c>
-      <c r="F16" s="117" t="s">
+      <c r="F16" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G16" s="103" t="s">
+      <c r="G16" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H16" s="109" t="s">
+      <c r="H16" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I16" s="118" t="s">
+      <c r="I16" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J16" s="101" t="s">
+      <c r="J16" s="91" t="s">
         <v>862</v>
       </c>
       <c r="K16" s="60"/>
@@ -29938,34 +30292,34 @@
       <c r="Z16" s="60"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="83" t="s">
         <v>867</v>
       </c>
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="97" t="s">
         <v>868</v>
       </c>
-      <c r="C17" s="108" t="s">
+      <c r="C17" s="98" t="s">
         <v>869</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="D17" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E17" s="101" t="s">
+      <c r="E17" s="91" t="s">
         <v>870</v>
       </c>
-      <c r="F17" s="125" t="s">
+      <c r="F17" s="115" t="s">
         <v>258</v>
       </c>
-      <c r="G17" s="103" t="s">
+      <c r="G17" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H17" s="109" t="s">
+      <c r="H17" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I17" s="118" t="s">
+      <c r="I17" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J17" s="126" t="s">
+      <c r="J17" s="116" t="s">
         <v>871</v>
       </c>
       <c r="K17" s="60"/>
@@ -29986,34 +30340,34 @@
       <c r="Z17" s="60"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="83" t="s">
         <v>872</v>
       </c>
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="97" t="s">
         <v>873</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="98" t="s">
         <v>874</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E18" s="101" t="s">
+      <c r="E18" s="91" t="s">
         <v>875</v>
       </c>
-      <c r="F18" s="117" t="s">
+      <c r="F18" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G18" s="103" t="s">
+      <c r="G18" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H18" s="109" t="s">
+      <c r="H18" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I18" s="118" t="s">
+      <c r="I18" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J18" s="101" t="s">
+      <c r="J18" s="91" t="s">
         <v>836</v>
       </c>
       <c r="K18" s="60"/>
@@ -30034,34 +30388,34 @@
       <c r="Z18" s="60"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="83" t="s">
         <v>876</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="97" t="s">
         <v>877</v>
       </c>
-      <c r="C19" s="108" t="s">
+      <c r="C19" s="98" t="s">
         <v>878</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E19" s="101" t="s">
+      <c r="E19" s="91" t="s">
         <v>879</v>
       </c>
-      <c r="F19" s="117" t="s">
+      <c r="F19" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G19" s="103" t="s">
+      <c r="G19" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H19" s="109" t="s">
+      <c r="H19" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I19" s="118" t="s">
+      <c r="I19" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J19" s="101" t="s">
+      <c r="J19" s="91" t="s">
         <v>862</v>
       </c>
       <c r="K19" s="60"/>
@@ -30082,34 +30436,34 @@
       <c r="Z19" s="60"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="83" t="s">
         <v>880</v>
       </c>
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="97" t="s">
         <v>877</v>
       </c>
-      <c r="C20" s="127" t="s">
+      <c r="C20" s="117" t="s">
         <v>881</v>
       </c>
-      <c r="D20" s="101" t="s">
+      <c r="D20" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E20" s="101" t="s">
+      <c r="E20" s="91" t="s">
         <v>882</v>
       </c>
-      <c r="F20" s="117" t="s">
+      <c r="F20" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G20" s="103" t="s">
+      <c r="G20" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H20" s="109" t="s">
+      <c r="H20" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I20" s="118" t="s">
+      <c r="I20" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J20" s="101" t="s">
+      <c r="J20" s="91" t="s">
         <v>853</v>
       </c>
       <c r="K20" s="60"/>
@@ -30130,34 +30484,34 @@
       <c r="Z20" s="60"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="83" t="s">
         <v>883</v>
       </c>
-      <c r="B21" s="107" t="s">
+      <c r="B21" s="97" t="s">
         <v>877</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="98" t="s">
         <v>884</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="91" t="s">
         <v>885</v>
       </c>
-      <c r="F21" s="117" t="s">
+      <c r="F21" s="107" t="s">
         <v>830</v>
       </c>
-      <c r="G21" s="103" t="s">
+      <c r="G21" s="93" t="s">
         <v>818</v>
       </c>
-      <c r="H21" s="109" t="s">
+      <c r="H21" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="I21" s="118" t="s">
+      <c r="I21" s="108" t="s">
         <v>254</v>
       </c>
-      <c r="J21" s="124" t="s">
+      <c r="J21" s="114" t="s">
         <v>255</v>
       </c>
       <c r="K21" s="60"/>

</xml_diff>

<commit_message>
Transfer request test case
</commit_message>
<xml_diff>
--- a/Test Case In Managerium.xlsx
+++ b/Test Case In Managerium.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="951">
   <si>
     <t>Product Name</t>
   </si>
@@ -3638,6 +3638,105 @@
   <si>
     <t xml:space="preserve">it will should be successfully shwoing PO and GRN in pending bill
 </t>
+  </si>
+  <si>
+    <r>
+      <t>MGM-8826</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Transfer Order from Available Stock</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create a New item.
+</t>
+  </si>
+  <si>
+    <t>Configuration-&gt;Item profile-&gt;add item</t>
+  </si>
+  <si>
+    <t>it will should be successfully Create item</t>
+  </si>
+  <si>
+    <t>purchase rececive</t>
+  </si>
+  <si>
+    <t>TC_148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to direct purchase rececive New item.
+</t>
+  </si>
+  <si>
+    <t>purchase -&gt;purchase rececive-&gt;Direct Receive</t>
+  </si>
+  <si>
+    <t>it will should be successfully direct purchase rececive New item.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer Request
+</t>
+  </si>
+  <si>
+    <t>TC_149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create Transfer Request 
+New item.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory-&gt; "Transfer Request-&gt; create Transfer Request
+</t>
+  </si>
+  <si>
+    <t>it will should be showing Available Stock in new item</t>
+  </si>
+  <si>
+    <t>TC_150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create Transfer Request
+New item Available Stock more transfer request
+</t>
+  </si>
+  <si>
+    <t>it will should be Available Stock more item try to transfer , approve time can not not approve tramsfer request.</t>
+  </si>
+  <si>
+    <t>TC_151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create Transfer Request New item Available Stock transfer request
+</t>
+  </si>
+  <si>
+    <t>it will should be Available Stock item try to transfer , approve time it can approve tramsfer request.</t>
+  </si>
+  <si>
+    <t>TC_152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to Create Direct Transfer New item Available Stock item more QTY transfer 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory-&gt; "Transfer -&gt; create Direct Transfer 
+</t>
+  </si>
+  <si>
+    <t>it will should be Available Stock more item try to Direct transfer time can not doing direct tramsfer .</t>
   </si>
 </sst>
 </file>
@@ -4562,32 +4661,32 @@
     <xf numFmtId="0" fontId="33" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4811,8 +4910,8 @@
   </sheetPr>
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S157" sqref="S157"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O158" sqref="O158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2"/>
@@ -4827,11 +4926,11 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="15"/>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="119"/>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="123" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="119"/>
@@ -4839,11 +4938,11 @@
         <v>2</v>
       </c>
       <c r="G1" s="119"/>
-      <c r="H1" s="124">
+      <c r="H1" s="127">
         <v>45615</v>
       </c>
       <c r="I1" s="119"/>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="125" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="119"/>
@@ -4859,11 +4958,11 @@
     </row>
     <row r="2" spans="1:26" ht="13.8">
       <c r="A2" s="15"/>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="126" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="119"/>
-      <c r="D2" s="121" t="s">
+      <c r="D2" s="123" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="119"/>
@@ -4871,14 +4970,14 @@
         <v>7</v>
       </c>
       <c r="G2" s="119"/>
-      <c r="H2" s="123"/>
+      <c r="H2" s="121"/>
       <c r="I2" s="119"/>
       <c r="J2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="19">
         <f>COUNTIF(M8:M1823,"Pass")</f>
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>9</v>
@@ -4892,15 +4991,15 @@
     </row>
     <row r="3" spans="1:26" ht="13.8">
       <c r="A3" s="15"/>
-      <c r="B3" s="126"/>
+      <c r="B3" s="120"/>
       <c r="C3" s="119"/>
-      <c r="D3" s="123"/>
+      <c r="D3" s="121"/>
       <c r="E3" s="119"/>
       <c r="F3" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="119"/>
-      <c r="H3" s="123"/>
+      <c r="H3" s="121"/>
       <c r="I3" s="119"/>
       <c r="J3" s="21" t="s">
         <v>11</v>
@@ -4921,11 +5020,11 @@
     </row>
     <row r="4" spans="1:26" ht="171.6">
       <c r="A4" s="15"/>
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="126" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="119"/>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="123" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="119"/>
@@ -4933,7 +5032,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="119"/>
-      <c r="H4" s="127"/>
+      <c r="H4" s="124"/>
       <c r="I4" s="119"/>
       <c r="J4" s="18" t="s">
         <v>16</v>
@@ -4954,11 +5053,11 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="15"/>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="126" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="119"/>
-      <c r="D5" s="121" t="s">
+      <c r="D5" s="123" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="119"/>
@@ -4966,7 +5065,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="119"/>
-      <c r="H5" s="123" t="s">
+      <c r="H5" s="121" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="119"/>
@@ -4975,7 +5074,7 @@
       </c>
       <c r="K5" s="26">
         <f>SUM(K2+K3+K4)</f>
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="L5" s="20" t="s">
         <v>23</v>
@@ -4990,7 +5089,7 @@
     <row r="6" spans="1:26">
       <c r="A6" s="27"/>
       <c r="B6" s="27"/>
-      <c r="C6" s="125"/>
+      <c r="C6" s="118"/>
       <c r="D6" s="119"/>
       <c r="E6" s="119"/>
       <c r="F6" s="119"/>
@@ -12401,120 +12500,240 @@
       <c r="Q158" s="4"/>
       <c r="R158" s="4"/>
     </row>
-    <row r="159" spans="1:18">
-      <c r="A159" s="4"/>
-      <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
-      <c r="E159" s="4"/>
-      <c r="F159" s="4"/>
-      <c r="G159" s="4"/>
-      <c r="H159" s="4"/>
-      <c r="I159" s="4"/>
-      <c r="J159" s="4"/>
-      <c r="K159" s="4"/>
-      <c r="L159" s="4"/>
-      <c r="M159" s="4"/>
+    <row r="159" spans="1:18" ht="66.599999999999994" thickBot="1">
+      <c r="A159" s="70"/>
+      <c r="B159" s="69" t="s">
+        <v>926</v>
+      </c>
+      <c r="C159" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="D159" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E159" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="F159" s="30" t="s">
+        <v>928</v>
+      </c>
+      <c r="G159" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="H159" s="30" t="s">
+        <v>929</v>
+      </c>
+      <c r="I159" s="30"/>
+      <c r="J159" s="30"/>
+      <c r="K159" s="30" t="s">
+        <v>930</v>
+      </c>
+      <c r="L159" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="M159" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="N159" s="4"/>
       <c r="O159" s="4"/>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
       <c r="R159" s="4"/>
     </row>
-    <row r="160" spans="1:18">
-      <c r="A160" s="4"/>
-      <c r="B160" s="4"/>
-      <c r="C160" s="4"/>
-      <c r="D160" s="4"/>
-      <c r="E160" s="4"/>
-      <c r="F160" s="4"/>
-      <c r="G160" s="4"/>
-      <c r="H160" s="4"/>
-      <c r="I160" s="4"/>
-      <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
-      <c r="L160" s="4"/>
-      <c r="M160" s="4"/>
+    <row r="160" spans="1:18" ht="93" thickBot="1">
+      <c r="A160" s="35"/>
+      <c r="B160" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="C160" s="36" t="s">
+        <v>931</v>
+      </c>
+      <c r="D160" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E160" s="38" t="s">
+        <v>932</v>
+      </c>
+      <c r="F160" s="36" t="s">
+        <v>933</v>
+      </c>
+      <c r="G160" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H160" s="36" t="s">
+        <v>934</v>
+      </c>
+      <c r="I160" s="36"/>
+      <c r="J160" s="36"/>
+      <c r="K160" s="36" t="s">
+        <v>935</v>
+      </c>
+      <c r="L160" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M160" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N160" s="4"/>
       <c r="O160" s="4"/>
       <c r="P160" s="4"/>
       <c r="Q160" s="4"/>
       <c r="R160" s="4"/>
     </row>
-    <row r="161" spans="1:18">
-      <c r="A161" s="4"/>
-      <c r="B161" s="4"/>
-      <c r="C161" s="4"/>
-      <c r="D161" s="4"/>
-      <c r="E161" s="4"/>
-      <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
-      <c r="H161" s="4"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
-      <c r="L161" s="4"/>
-      <c r="M161" s="4"/>
+    <row r="161" spans="1:18" ht="66.599999999999994" thickBot="1">
+      <c r="A161" s="35"/>
+      <c r="B161" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="C161" s="36" t="s">
+        <v>936</v>
+      </c>
+      <c r="D161" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E161" s="38" t="s">
+        <v>937</v>
+      </c>
+      <c r="F161" s="36" t="s">
+        <v>938</v>
+      </c>
+      <c r="G161" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H161" s="36" t="s">
+        <v>939</v>
+      </c>
+      <c r="I161" s="36"/>
+      <c r="J161" s="36"/>
+      <c r="K161" s="36" t="s">
+        <v>940</v>
+      </c>
+      <c r="L161" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M161" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N161" s="4"/>
       <c r="O161" s="4"/>
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
       <c r="R161" s="4"/>
     </row>
-    <row r="162" spans="1:18">
-      <c r="A162" s="4"/>
-      <c r="B162" s="4"/>
-      <c r="C162" s="4"/>
-      <c r="D162" s="4"/>
-      <c r="E162" s="4"/>
-      <c r="F162" s="4"/>
-      <c r="G162" s="4"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
+    <row r="162" spans="1:18" ht="132.6" thickBot="1">
+      <c r="A162" s="35"/>
+      <c r="B162" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="C162" s="36" t="s">
+        <v>936</v>
+      </c>
+      <c r="D162" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E162" s="38" t="s">
+        <v>941</v>
+      </c>
+      <c r="F162" s="36" t="s">
+        <v>942</v>
+      </c>
+      <c r="G162" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H162" s="36" t="s">
+        <v>939</v>
+      </c>
+      <c r="I162" s="36"/>
+      <c r="J162" s="36"/>
+      <c r="K162" s="36" t="s">
+        <v>943</v>
+      </c>
+      <c r="L162" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M162" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N162" s="4"/>
       <c r="O162" s="4"/>
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
       <c r="R162" s="4"/>
     </row>
-    <row r="163" spans="1:18">
-      <c r="A163" s="4"/>
-      <c r="B163" s="4"/>
-      <c r="C163" s="4"/>
-      <c r="D163" s="4"/>
-      <c r="E163" s="4"/>
-      <c r="F163" s="4"/>
-      <c r="G163" s="4"/>
-      <c r="H163" s="4"/>
-      <c r="I163" s="4"/>
-      <c r="J163" s="4"/>
-      <c r="K163" s="4"/>
-      <c r="L163" s="4"/>
-      <c r="M163" s="4"/>
+    <row r="163" spans="1:18" ht="106.2" thickBot="1">
+      <c r="A163" s="35"/>
+      <c r="B163" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="C163" s="36" t="s">
+        <v>936</v>
+      </c>
+      <c r="D163" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E163" s="38" t="s">
+        <v>944</v>
+      </c>
+      <c r="F163" s="36" t="s">
+        <v>945</v>
+      </c>
+      <c r="G163" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H163" s="36" t="s">
+        <v>939</v>
+      </c>
+      <c r="I163" s="36"/>
+      <c r="J163" s="36"/>
+      <c r="K163" s="36" t="s">
+        <v>946</v>
+      </c>
+      <c r="L163" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M163" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N163" s="4"/>
       <c r="O163" s="4"/>
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
       <c r="R163" s="4"/>
     </row>
-    <row r="164" spans="1:18">
-      <c r="A164" s="4"/>
-      <c r="B164" s="4"/>
-      <c r="C164" s="4"/>
-      <c r="D164" s="4"/>
-      <c r="E164" s="4"/>
-      <c r="F164" s="4"/>
-      <c r="G164" s="4"/>
-      <c r="H164" s="4"/>
-      <c r="I164" s="4"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
-      <c r="L164" s="4"/>
-      <c r="M164" s="4"/>
+    <row r="164" spans="1:18" ht="119.4" thickBot="1">
+      <c r="A164" s="35"/>
+      <c r="B164" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="C164" s="36" t="s">
+        <v>936</v>
+      </c>
+      <c r="D164" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E164" s="38" t="s">
+        <v>947</v>
+      </c>
+      <c r="F164" s="36" t="s">
+        <v>948</v>
+      </c>
+      <c r="G164" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="H164" s="36" t="s">
+        <v>949</v>
+      </c>
+      <c r="I164" s="36"/>
+      <c r="J164" s="36"/>
+      <c r="K164" s="36" t="s">
+        <v>950</v>
+      </c>
+      <c r="L164" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M164" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="N164" s="4"/>
       <c r="O164" s="4"/>
       <c r="P164" s="4"/>
@@ -29343,14 +29562,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -29365,6 +29576,14 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="M8">
@@ -29502,9 +29721,15 @@
     <hyperlink ref="B157" r:id="rId125" display="https://jira.ibos.io/browse/MGM-8602"/>
     <hyperlink ref="B158" r:id="rId126" display="https://jira.ibos.io/browse/MGM-8602"/>
     <hyperlink ref="J158" r:id="rId127"/>
+    <hyperlink ref="B159" r:id="rId128" display="https://jira.ibos.io/browse/MGM-8826"/>
+    <hyperlink ref="B160" r:id="rId129" display="https://jira.ibos.io/browse/MGM-8826"/>
+    <hyperlink ref="B161" r:id="rId130" display="https://jira.ibos.io/browse/MGM-8826"/>
+    <hyperlink ref="B162" r:id="rId131" display="https://jira.ibos.io/browse/MGM-8826"/>
+    <hyperlink ref="B163" r:id="rId132" display="https://jira.ibos.io/browse/MGM-8826"/>
+    <hyperlink ref="B164" r:id="rId133" display="https://jira.ibos.io/browse/MGM-8826"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId128"/>
+  <pageSetup orientation="portrait" r:id="rId134"/>
 </worksheet>
 </file>
 

</xml_diff>